<commit_message>
Add more data to test.xlsx
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brandontorres\PycharmProjects\csc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="1875" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="1875" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Schools" sheetId="2" r:id="rId1"/>
-    <sheet name="Clubs" sheetId="3" r:id="rId2"/>
+    <sheet name="Users" sheetId="4" r:id="rId2"/>
+    <sheet name="Clubs" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="286">
   <si>
     <t>Avila University</t>
   </si>
@@ -709,6 +710,180 @@
   </si>
   <si>
     <t>Water &amp; Environmental Technologists (WET)</t>
+  </si>
+  <si>
+    <t>Vance Lemoine  </t>
+  </si>
+  <si>
+    <t>Valencia Tripodi  </t>
+  </si>
+  <si>
+    <t>Estelle Oram  </t>
+  </si>
+  <si>
+    <t>Cornelius Bomberger  </t>
+  </si>
+  <si>
+    <t>Karyl Horvat  </t>
+  </si>
+  <si>
+    <t>Delfina Wescott  </t>
+  </si>
+  <si>
+    <t>Albina Hudak  </t>
+  </si>
+  <si>
+    <t>Alicia Sayles  </t>
+  </si>
+  <si>
+    <t>Sade Berney  </t>
+  </si>
+  <si>
+    <t>Royal Perales  </t>
+  </si>
+  <si>
+    <t>Moshe Waage  </t>
+  </si>
+  <si>
+    <t>Devon Mcgurk  </t>
+  </si>
+  <si>
+    <t>Kaila Blow  </t>
+  </si>
+  <si>
+    <t>Kermit Valladares  </t>
+  </si>
+  <si>
+    <t>Tristan Crigler  </t>
+  </si>
+  <si>
+    <t>Del Innis  </t>
+  </si>
+  <si>
+    <t>Amy Astin  </t>
+  </si>
+  <si>
+    <t>Elois Nevarez  </t>
+  </si>
+  <si>
+    <t>Kit Romain  </t>
+  </si>
+  <si>
+    <t>Palma Boldt  </t>
+  </si>
+  <si>
+    <t>Lauralee Shewmake  </t>
+  </si>
+  <si>
+    <t>Zaida Lisle  </t>
+  </si>
+  <si>
+    <t>Kerrie Lease  </t>
+  </si>
+  <si>
+    <t>Vito Striplin  </t>
+  </si>
+  <si>
+    <t>Xuan Michelson  </t>
+  </si>
+  <si>
+    <t>Bettyann Julien  </t>
+  </si>
+  <si>
+    <t>Niki Beecher  </t>
+  </si>
+  <si>
+    <t>Saturnina Gandhi  </t>
+  </si>
+  <si>
+    <t>Hubert Stott  </t>
+  </si>
+  <si>
+    <t>Odis Pattison  </t>
+  </si>
+  <si>
+    <t>Carmelia Brock  </t>
+  </si>
+  <si>
+    <t>Lacey Corman  </t>
+  </si>
+  <si>
+    <t>Denyse Peavler  </t>
+  </si>
+  <si>
+    <t>Regine Rivenburg  </t>
+  </si>
+  <si>
+    <t>Arleen Samons  </t>
+  </si>
+  <si>
+    <t>Mindy Stearman  </t>
+  </si>
+  <si>
+    <t>Henrietta Wolken  </t>
+  </si>
+  <si>
+    <t>Jenae Hamm  </t>
+  </si>
+  <si>
+    <t>Pete Pendergraft  </t>
+  </si>
+  <si>
+    <t>Tad Anderton  </t>
+  </si>
+  <si>
+    <t>Vince Sunderman  </t>
+  </si>
+  <si>
+    <t>Virgie Hipple  </t>
+  </si>
+  <si>
+    <t>Ashley Gitlin  </t>
+  </si>
+  <si>
+    <t>Julia Denner  </t>
+  </si>
+  <si>
+    <t>Elana Cuffee  </t>
+  </si>
+  <si>
+    <t>Rozanne Garden  </t>
+  </si>
+  <si>
+    <t>Salley Quiroz  </t>
+  </si>
+  <si>
+    <t>Ozell Costas  </t>
+  </si>
+  <si>
+    <t>Vivienne Hardee  </t>
+  </si>
+  <si>
+    <t>Shawnee Driskill  </t>
+  </si>
+  <si>
+    <t>member</t>
+  </si>
+  <si>
+    <t>GM</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>Universe</t>
+  </si>
+  <si>
+    <t>Tesla</t>
+  </si>
+  <si>
+    <t>competition Host</t>
+  </si>
+  <si>
+    <t>ASME National</t>
+  </si>
+  <si>
+    <t>AIAA National</t>
   </si>
 </sst>
 </file>
@@ -1062,7 +1237,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C113"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -2322,13 +2497,1118 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E55"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B1" t="str">
+        <f ca="1">CHOOSE(RAND()*3+1,"Engineering","Communication","Business")</f>
+        <v>Business</v>
+      </c>
+      <c r="C1" t="str">
+        <f ca="1">CHOOSE(RAND()*3+1,"California","Missouri","Florida")</f>
+        <v>Florida</v>
+      </c>
+      <c r="D1" t="str">
+        <f ca="1">CHOOSE(RAND()*3+1,"Pensacola","Springfield","Las Vegas")</f>
+        <v>Las Vegas</v>
+      </c>
+      <c r="E1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B2" t="str">
+        <f t="shared" ref="B2:B50" ca="1" si="0">CHOOSE(RAND()*3+1,"Engineering","Communication","Business")</f>
+        <v>Engineering</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C55" ca="1" si="1">CHOOSE(RAND()*3+1,"California","Missouri","Florida")</f>
+        <v>Missouri</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D55" ca="1" si="2">CHOOSE(RAND()*3+1,"Pensacola","Springfield","Las Vegas")</f>
+        <v>Pensacola</v>
+      </c>
+      <c r="E2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Communication</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Missouri</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Springfield</v>
+      </c>
+      <c r="E3" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>231</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Engineering</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>California</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Pensacola</v>
+      </c>
+      <c r="E4" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>232</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Communication</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>California</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Las Vegas</v>
+      </c>
+      <c r="E5" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>233</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Engineering</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>California</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Pensacola</v>
+      </c>
+      <c r="E6" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>234</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Communication</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>California</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Springfield</v>
+      </c>
+      <c r="E7" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>235</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Engineering</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Florida</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Pensacola</v>
+      </c>
+      <c r="E8" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>236</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Business</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>California</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Pensacola</v>
+      </c>
+      <c r="E9" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>237</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Engineering</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>California</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Pensacola</v>
+      </c>
+      <c r="E10" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>238</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Communication</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Missouri</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Pensacola</v>
+      </c>
+      <c r="E11" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>239</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Communication</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Florida</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Pensacola</v>
+      </c>
+      <c r="E12" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>240</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Communication</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>California</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Pensacola</v>
+      </c>
+      <c r="E13" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>241</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Engineering</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Missouri</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Las Vegas</v>
+      </c>
+      <c r="E14" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>242</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Engineering</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>California</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Springfield</v>
+      </c>
+      <c r="E15" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>243</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Engineering</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Florida</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Springfield</v>
+      </c>
+      <c r="E16" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>244</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Business</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>California</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Springfield</v>
+      </c>
+      <c r="E17" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>245</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Communication</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>California</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Springfield</v>
+      </c>
+      <c r="E18" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>246</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Engineering</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Florida</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Las Vegas</v>
+      </c>
+      <c r="E19" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>247</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Communication</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Florida</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Springfield</v>
+      </c>
+      <c r="E20" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>248</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Engineering</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Florida</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Las Vegas</v>
+      </c>
+      <c r="E21" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>249</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Business</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>California</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Pensacola</v>
+      </c>
+      <c r="E22" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>250</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Business</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Florida</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Las Vegas</v>
+      </c>
+      <c r="E23" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>251</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Communication</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>California</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Springfield</v>
+      </c>
+      <c r="E24" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>252</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Communication</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Florida</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Pensacola</v>
+      </c>
+      <c r="E25" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>253</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Engineering</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Florida</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Pensacola</v>
+      </c>
+      <c r="E26" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>254</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Engineering</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Missouri</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Springfield</v>
+      </c>
+      <c r="E27" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>255</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Engineering</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>California</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Pensacola</v>
+      </c>
+      <c r="E28" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>256</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Communication</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Florida</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Pensacola</v>
+      </c>
+      <c r="E29" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>257</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Business</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>California</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Springfield</v>
+      </c>
+      <c r="E30" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>258</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Communication</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>California</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Springfield</v>
+      </c>
+      <c r="E31" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>259</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Business</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>California</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Pensacola</v>
+      </c>
+      <c r="E32" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>260</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Business</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Florida</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Springfield</v>
+      </c>
+      <c r="E33" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>261</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Communication</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>California</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Las Vegas</v>
+      </c>
+      <c r="E34" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>262</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Engineering</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Missouri</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Springfield</v>
+      </c>
+      <c r="E35" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>263</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Communication</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Florida</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Pensacola</v>
+      </c>
+      <c r="E36" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>264</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Business</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Missouri</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Springfield</v>
+      </c>
+      <c r="E37" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>265</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Communication</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Missouri</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Pensacola</v>
+      </c>
+      <c r="E38" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>266</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Business</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>California</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Las Vegas</v>
+      </c>
+      <c r="E39" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>267</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Engineering</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Missouri</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Springfield</v>
+      </c>
+      <c r="E40" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>268</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Engineering</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Missouri</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Pensacola</v>
+      </c>
+      <c r="E41" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>269</v>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Business</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Florida</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Springfield</v>
+      </c>
+      <c r="E42" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>270</v>
+      </c>
+      <c r="B43" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Engineering</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Missouri</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Las Vegas</v>
+      </c>
+      <c r="E43" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>271</v>
+      </c>
+      <c r="B44" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Engineering</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Florida</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Pensacola</v>
+      </c>
+      <c r="E44" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>272</v>
+      </c>
+      <c r="B45" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Business</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Florida</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Pensacola</v>
+      </c>
+      <c r="E45" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>273</v>
+      </c>
+      <c r="B46" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Engineering</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>California</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Las Vegas</v>
+      </c>
+      <c r="E46" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>274</v>
+      </c>
+      <c r="B47" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Communication</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>California</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Springfield</v>
+      </c>
+      <c r="E47" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>275</v>
+      </c>
+      <c r="B48" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Engineering</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Missouri</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Las Vegas</v>
+      </c>
+      <c r="E48" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>276</v>
+      </c>
+      <c r="B49" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Engineering</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Florida</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Las Vegas</v>
+      </c>
+      <c r="E49" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>277</v>
+      </c>
+      <c r="B50" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Communication</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Florida</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Springfield</v>
+      </c>
+      <c r="E50" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>279</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>California</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Springfield</v>
+      </c>
+      <c r="E51" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>281</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Missouri</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Las Vegas</v>
+      </c>
+      <c r="E52" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>282</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>California</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Pensacola</v>
+      </c>
+      <c r="E53" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>284</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Florida</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Springfield</v>
+      </c>
+      <c r="E54" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>285</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>California</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Las Vegas</v>
+      </c>
+      <c r="E55" t="s">
+        <v>283</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="57.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Switch from Peewee to Pony
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,16 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brandontorres\PycharmProjects\csc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\brandon\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="1875" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="1875" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Schools" sheetId="2" r:id="rId1"/>
-    <sheet name="Users" sheetId="4" r:id="rId2"/>
-    <sheet name="Clubs" sheetId="3" r:id="rId3"/>
+    <sheet name="School" sheetId="2" r:id="rId1"/>
+    <sheet name="Member" sheetId="4" r:id="rId2"/>
+    <sheet name="Club" sheetId="3" r:id="rId3"/>
+    <sheet name="Company" sheetId="5" r:id="rId4"/>
+    <sheet name="CompetitionHost" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="290">
   <si>
     <t>Avila University</t>
   </si>
@@ -862,28 +864,40 @@
     <t>Shawnee Driskill  </t>
   </si>
   <si>
-    <t>member</t>
-  </si>
-  <si>
     <t>GM</t>
   </si>
   <si>
-    <t>company</t>
-  </si>
-  <si>
     <t>Universe</t>
   </si>
   <si>
     <t>Tesla</t>
   </si>
   <si>
-    <t>competition Host</t>
-  </si>
-  <si>
     <t>ASME National</t>
   </si>
   <si>
     <t>AIAA National</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>Las Vegas</t>
+  </si>
+  <si>
+    <t>Engineering</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>Pensacola</t>
+  </si>
+  <si>
+    <t>Communication</t>
   </si>
 </sst>
 </file>
@@ -1237,9 +1251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C113"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView topLeftCell="A87" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1251,8 +1263,9 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
+      <c r="B1" t="str">
+        <f ca="1">INDEX(A5:A12,RAND()*10+0.5)</f>
+        <v>Central Methodist University College of Liberal Arts &amp; Sciences</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -2497,1099 +2510,869 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" customWidth="1"/>
+    <col min="5" max="5" width="62" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>228</v>
       </c>
-      <c r="B1" t="str">
-        <f ca="1">CHOOSE(RAND()*3+1,"Engineering","Communication","Business")</f>
-        <v>Business</v>
-      </c>
-      <c r="C1" t="str">
-        <f ca="1">CHOOSE(RAND()*3+1,"California","Missouri","Florida")</f>
-        <v>Florida</v>
-      </c>
-      <c r="D1" t="str">
-        <f ca="1">CHOOSE(RAND()*3+1,"Pensacola","Springfield","Las Vegas")</f>
-        <v>Las Vegas</v>
+      <c r="B1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>278</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>229</v>
       </c>
-      <c r="B2" t="str">
-        <f t="shared" ref="B2:B50" ca="1" si="0">CHOOSE(RAND()*3+1,"Engineering","Communication","Business")</f>
-        <v>Engineering</v>
-      </c>
-      <c r="C2" t="str">
-        <f t="shared" ref="C2:C55" ca="1" si="1">CHOOSE(RAND()*3+1,"California","Missouri","Florida")</f>
-        <v>Missouri</v>
-      </c>
-      <c r="D2" t="str">
-        <f t="shared" ref="D2:D55" ca="1" si="2">CHOOSE(RAND()*3+1,"Pensacola","Springfield","Las Vegas")</f>
-        <v>Pensacola</v>
+      <c r="B2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>283</v>
       </c>
       <c r="E2" t="s">
-        <v>278</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>230</v>
       </c>
-      <c r="B3" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Communication</v>
-      </c>
-      <c r="C3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Missouri</v>
-      </c>
-      <c r="D3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Springfield</v>
+      <c r="B3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>287</v>
       </c>
       <c r="E3" t="s">
-        <v>278</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>231</v>
       </c>
-      <c r="B4" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Engineering</v>
-      </c>
-      <c r="C4" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>California</v>
-      </c>
-      <c r="D4" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Pensacola</v>
+      <c r="B4" t="s">
+        <v>286</v>
+      </c>
+      <c r="C4" t="s">
+        <v>288</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>278</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>232</v>
       </c>
-      <c r="B5" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Communication</v>
-      </c>
-      <c r="C5" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>California</v>
-      </c>
-      <c r="D5" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Las Vegas</v>
+      <c r="B5" t="s">
+        <v>289</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>287</v>
       </c>
       <c r="E5" t="s">
-        <v>278</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>233</v>
       </c>
-      <c r="B6" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Engineering</v>
-      </c>
-      <c r="C6" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>California</v>
-      </c>
-      <c r="D6" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Pensacola</v>
+      <c r="B6" t="s">
+        <v>285</v>
+      </c>
+      <c r="C6" t="s">
+        <v>288</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>278</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>234</v>
       </c>
-      <c r="B7" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Communication</v>
-      </c>
-      <c r="C7" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>California</v>
-      </c>
-      <c r="D7" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Springfield</v>
+      <c r="B7" t="s">
+        <v>289</v>
+      </c>
+      <c r="C7" t="s">
+        <v>284</v>
+      </c>
+      <c r="D7" t="s">
+        <v>287</v>
       </c>
       <c r="E7" t="s">
-        <v>278</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>235</v>
       </c>
-      <c r="B8" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Engineering</v>
-      </c>
-      <c r="C8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Florida</v>
-      </c>
-      <c r="D8" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Pensacola</v>
+      <c r="B8" t="s">
+        <v>285</v>
+      </c>
+      <c r="C8" t="s">
+        <v>284</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>278</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>236</v>
       </c>
-      <c r="B9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Business</v>
-      </c>
-      <c r="C9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>California</v>
-      </c>
-      <c r="D9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Pensacola</v>
+      <c r="B9" t="s">
+        <v>289</v>
+      </c>
+      <c r="C9" t="s">
+        <v>284</v>
+      </c>
+      <c r="D9" t="s">
+        <v>283</v>
       </c>
       <c r="E9" t="s">
-        <v>278</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>237</v>
       </c>
-      <c r="B10" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Engineering</v>
-      </c>
-      <c r="C10" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>California</v>
-      </c>
-      <c r="D10" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Pensacola</v>
+      <c r="B10" t="s">
+        <v>286</v>
+      </c>
+      <c r="C10" t="s">
+        <v>284</v>
+      </c>
+      <c r="D10" t="s">
+        <v>283</v>
       </c>
       <c r="E10" t="s">
-        <v>278</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>238</v>
       </c>
-      <c r="B11" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Communication</v>
-      </c>
-      <c r="C11" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Missouri</v>
-      </c>
-      <c r="D11" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Pensacola</v>
+      <c r="B11" t="s">
+        <v>289</v>
+      </c>
+      <c r="C11" t="s">
+        <v>284</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>278</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>239</v>
       </c>
-      <c r="B12" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Communication</v>
-      </c>
-      <c r="C12" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Florida</v>
-      </c>
-      <c r="D12" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Pensacola</v>
+      <c r="B12" t="s">
+        <v>286</v>
+      </c>
+      <c r="C12" t="s">
+        <v>288</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>278</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>240</v>
       </c>
-      <c r="B13" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Communication</v>
-      </c>
-      <c r="C13" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>California</v>
-      </c>
-      <c r="D13" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Pensacola</v>
+      <c r="B13" t="s">
+        <v>289</v>
+      </c>
+      <c r="C13" t="s">
+        <v>288</v>
+      </c>
+      <c r="D13" t="s">
+        <v>283</v>
       </c>
       <c r="E13" t="s">
-        <v>278</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>241</v>
       </c>
-      <c r="B14" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Engineering</v>
-      </c>
-      <c r="C14" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Missouri</v>
-      </c>
-      <c r="D14" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Las Vegas</v>
+      <c r="B14" t="s">
+        <v>285</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>283</v>
       </c>
       <c r="E14" t="s">
-        <v>278</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>242</v>
       </c>
-      <c r="B15" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Engineering</v>
-      </c>
-      <c r="C15" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>California</v>
-      </c>
-      <c r="D15" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Springfield</v>
+      <c r="B15" t="s">
+        <v>289</v>
+      </c>
+      <c r="C15" t="s">
+        <v>288</v>
+      </c>
+      <c r="D15" t="s">
+        <v>287</v>
       </c>
       <c r="E15" t="s">
-        <v>278</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>243</v>
       </c>
-      <c r="B16" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Engineering</v>
-      </c>
-      <c r="C16" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Florida</v>
-      </c>
-      <c r="D16" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Springfield</v>
+      <c r="B16" t="s">
+        <v>285</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>278</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>244</v>
       </c>
-      <c r="B17" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Business</v>
-      </c>
-      <c r="C17" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>California</v>
-      </c>
-      <c r="D17" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Springfield</v>
+      <c r="B17" t="s">
+        <v>285</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>287</v>
       </c>
       <c r="E17" t="s">
-        <v>278</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>245</v>
       </c>
-      <c r="B18" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Communication</v>
-      </c>
-      <c r="C18" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>California</v>
-      </c>
-      <c r="D18" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Springfield</v>
+      <c r="B18" t="s">
+        <v>286</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>278</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>246</v>
       </c>
-      <c r="B19" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Engineering</v>
-      </c>
-      <c r="C19" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Florida</v>
-      </c>
-      <c r="D19" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Las Vegas</v>
+      <c r="B19" t="s">
+        <v>286</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>283</v>
       </c>
       <c r="E19" t="s">
-        <v>278</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>247</v>
       </c>
-      <c r="B20" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Communication</v>
-      </c>
-      <c r="C20" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Florida</v>
-      </c>
-      <c r="D20" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Springfield</v>
+      <c r="B20" t="s">
+        <v>285</v>
+      </c>
+      <c r="C20" t="s">
+        <v>288</v>
+      </c>
+      <c r="D20" t="s">
+        <v>283</v>
       </c>
       <c r="E20" t="s">
-        <v>278</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>248</v>
       </c>
-      <c r="B21" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Engineering</v>
-      </c>
-      <c r="C21" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Florida</v>
-      </c>
-      <c r="D21" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Las Vegas</v>
+      <c r="B21" t="s">
+        <v>286</v>
+      </c>
+      <c r="C21" t="s">
+        <v>288</v>
+      </c>
+      <c r="D21" t="s">
+        <v>283</v>
       </c>
       <c r="E21" t="s">
-        <v>278</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>249</v>
       </c>
-      <c r="B22" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Business</v>
-      </c>
-      <c r="C22" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>California</v>
-      </c>
-      <c r="D22" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Pensacola</v>
+      <c r="B22" t="s">
+        <v>289</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>278</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>250</v>
       </c>
-      <c r="B23" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Business</v>
-      </c>
-      <c r="C23" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Florida</v>
-      </c>
-      <c r="D23" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Las Vegas</v>
+      <c r="B23" t="s">
+        <v>289</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2</v>
       </c>
       <c r="E23" t="s">
-        <v>278</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>251</v>
       </c>
-      <c r="B24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Communication</v>
-      </c>
-      <c r="C24" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>California</v>
-      </c>
-      <c r="D24" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Springfield</v>
+      <c r="B24" t="s">
+        <v>285</v>
+      </c>
+      <c r="C24" t="s">
+        <v>284</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>278</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>252</v>
       </c>
-      <c r="B25" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Communication</v>
-      </c>
-      <c r="C25" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Florida</v>
-      </c>
-      <c r="D25" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Pensacola</v>
+      <c r="B25" t="s">
+        <v>286</v>
+      </c>
+      <c r="C25" t="s">
+        <v>284</v>
+      </c>
+      <c r="D25" t="s">
+        <v>283</v>
       </c>
       <c r="E25" t="s">
-        <v>278</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>253</v>
       </c>
-      <c r="B26" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Engineering</v>
-      </c>
-      <c r="C26" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Florida</v>
-      </c>
-      <c r="D26" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Pensacola</v>
+      <c r="B26" t="s">
+        <v>285</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>287</v>
       </c>
       <c r="E26" t="s">
-        <v>278</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>254</v>
       </c>
-      <c r="B27" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Engineering</v>
-      </c>
-      <c r="C27" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Missouri</v>
-      </c>
-      <c r="D27" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Springfield</v>
+      <c r="B27" t="s">
+        <v>289</v>
+      </c>
+      <c r="C27" t="s">
+        <v>288</v>
+      </c>
+      <c r="D27" t="s">
+        <v>287</v>
       </c>
       <c r="E27" t="s">
-        <v>278</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>255</v>
       </c>
-      <c r="B28" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Engineering</v>
-      </c>
-      <c r="C28" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>California</v>
-      </c>
-      <c r="D28" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Pensacola</v>
+      <c r="B28" t="s">
+        <v>289</v>
+      </c>
+      <c r="C28" t="s">
+        <v>288</v>
+      </c>
+      <c r="D28" t="s">
+        <v>2</v>
       </c>
       <c r="E28" t="s">
-        <v>278</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>256</v>
       </c>
-      <c r="B29" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Communication</v>
-      </c>
-      <c r="C29" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Florida</v>
-      </c>
-      <c r="D29" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Pensacola</v>
+      <c r="B29" t="s">
+        <v>289</v>
+      </c>
+      <c r="C29" t="s">
+        <v>288</v>
+      </c>
+      <c r="D29" t="s">
+        <v>287</v>
       </c>
       <c r="E29" t="s">
-        <v>278</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>257</v>
       </c>
-      <c r="B30" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Business</v>
-      </c>
-      <c r="C30" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>California</v>
-      </c>
-      <c r="D30" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Springfield</v>
+      <c r="B30" t="s">
+        <v>285</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
+        <v>283</v>
       </c>
       <c r="E30" t="s">
-        <v>278</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>258</v>
       </c>
-      <c r="B31" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Communication</v>
-      </c>
-      <c r="C31" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>California</v>
-      </c>
-      <c r="D31" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Springfield</v>
+      <c r="B31" t="s">
+        <v>286</v>
+      </c>
+      <c r="C31" t="s">
+        <v>284</v>
+      </c>
+      <c r="D31" t="s">
+        <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>278</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>259</v>
       </c>
-      <c r="B32" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Business</v>
-      </c>
-      <c r="C32" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>California</v>
-      </c>
-      <c r="D32" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Pensacola</v>
+      <c r="B32" t="s">
+        <v>286</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" t="s">
+        <v>287</v>
       </c>
       <c r="E32" t="s">
-        <v>278</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>260</v>
       </c>
-      <c r="B33" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Business</v>
-      </c>
-      <c r="C33" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Florida</v>
-      </c>
-      <c r="D33" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Springfield</v>
+      <c r="B33" t="s">
+        <v>289</v>
+      </c>
+      <c r="C33" t="s">
+        <v>288</v>
+      </c>
+      <c r="D33" t="s">
+        <v>283</v>
       </c>
       <c r="E33" t="s">
-        <v>278</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>261</v>
       </c>
-      <c r="B34" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Communication</v>
-      </c>
-      <c r="C34" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>California</v>
-      </c>
-      <c r="D34" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Las Vegas</v>
+      <c r="B34" t="s">
+        <v>289</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>287</v>
       </c>
       <c r="E34" t="s">
-        <v>278</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>262</v>
       </c>
-      <c r="B35" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Engineering</v>
-      </c>
-      <c r="C35" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Missouri</v>
-      </c>
-      <c r="D35" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Springfield</v>
+      <c r="B35" t="s">
+        <v>285</v>
+      </c>
+      <c r="C35" t="s">
+        <v>288</v>
+      </c>
+      <c r="D35" t="s">
+        <v>283</v>
       </c>
       <c r="E35" t="s">
-        <v>278</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>263</v>
       </c>
-      <c r="B36" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Communication</v>
-      </c>
-      <c r="C36" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Florida</v>
-      </c>
-      <c r="D36" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Pensacola</v>
+      <c r="B36" t="s">
+        <v>286</v>
+      </c>
+      <c r="C36" t="s">
+        <v>284</v>
+      </c>
+      <c r="D36" t="s">
+        <v>287</v>
       </c>
       <c r="E36" t="s">
-        <v>278</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>264</v>
       </c>
-      <c r="B37" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Business</v>
-      </c>
-      <c r="C37" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Missouri</v>
-      </c>
-      <c r="D37" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Springfield</v>
+      <c r="B37" t="s">
+        <v>289</v>
+      </c>
+      <c r="C37" t="s">
+        <v>284</v>
+      </c>
+      <c r="D37" t="s">
+        <v>283</v>
       </c>
       <c r="E37" t="s">
-        <v>278</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>265</v>
       </c>
-      <c r="B38" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Communication</v>
-      </c>
-      <c r="C38" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Missouri</v>
-      </c>
-      <c r="D38" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Pensacola</v>
+      <c r="B38" t="s">
+        <v>286</v>
+      </c>
+      <c r="C38" t="s">
+        <v>284</v>
+      </c>
+      <c r="D38" t="s">
+        <v>287</v>
       </c>
       <c r="E38" t="s">
-        <v>278</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>266</v>
       </c>
-      <c r="B39" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Business</v>
-      </c>
-      <c r="C39" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>California</v>
-      </c>
-      <c r="D39" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Las Vegas</v>
+      <c r="B39" t="s">
+        <v>289</v>
+      </c>
+      <c r="C39" t="s">
+        <v>288</v>
+      </c>
+      <c r="D39" t="s">
+        <v>283</v>
       </c>
       <c r="E39" t="s">
-        <v>278</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>267</v>
       </c>
-      <c r="B40" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Engineering</v>
-      </c>
-      <c r="C40" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Missouri</v>
-      </c>
-      <c r="D40" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Springfield</v>
+      <c r="B40" t="s">
+        <v>286</v>
+      </c>
+      <c r="C40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" t="s">
+        <v>2</v>
       </c>
       <c r="E40" t="s">
-        <v>278</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>268</v>
       </c>
-      <c r="B41" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Engineering</v>
-      </c>
-      <c r="C41" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Missouri</v>
-      </c>
-      <c r="D41" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Pensacola</v>
+      <c r="B41" t="s">
+        <v>286</v>
+      </c>
+      <c r="C41" t="s">
+        <v>288</v>
+      </c>
+      <c r="D41" t="s">
+        <v>283</v>
       </c>
       <c r="E41" t="s">
-        <v>278</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>269</v>
       </c>
-      <c r="B42" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Business</v>
-      </c>
-      <c r="C42" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Florida</v>
-      </c>
-      <c r="D42" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Springfield</v>
+      <c r="B42" t="s">
+        <v>289</v>
+      </c>
+      <c r="C42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" t="s">
+        <v>287</v>
       </c>
       <c r="E42" t="s">
-        <v>278</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>270</v>
       </c>
-      <c r="B43" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Engineering</v>
-      </c>
-      <c r="C43" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Missouri</v>
-      </c>
-      <c r="D43" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Las Vegas</v>
+      <c r="B43" t="s">
+        <v>289</v>
+      </c>
+      <c r="C43" t="s">
+        <v>288</v>
+      </c>
+      <c r="D43" t="s">
+        <v>2</v>
       </c>
       <c r="E43" t="s">
-        <v>278</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>271</v>
       </c>
-      <c r="B44" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Engineering</v>
-      </c>
-      <c r="C44" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Florida</v>
-      </c>
-      <c r="D44" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Pensacola</v>
+      <c r="B44" t="s">
+        <v>289</v>
+      </c>
+      <c r="C44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" t="s">
+        <v>2</v>
       </c>
       <c r="E44" t="s">
-        <v>278</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>272</v>
       </c>
-      <c r="B45" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Business</v>
-      </c>
-      <c r="C45" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Florida</v>
-      </c>
-      <c r="D45" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Pensacola</v>
+      <c r="B45" t="s">
+        <v>289</v>
+      </c>
+      <c r="C45" t="s">
+        <v>284</v>
+      </c>
+      <c r="D45" t="s">
+        <v>283</v>
       </c>
       <c r="E45" t="s">
-        <v>278</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>273</v>
       </c>
-      <c r="B46" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Engineering</v>
-      </c>
-      <c r="C46" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>California</v>
-      </c>
-      <c r="D46" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Las Vegas</v>
+      <c r="B46" t="s">
+        <v>285</v>
+      </c>
+      <c r="C46" t="s">
+        <v>284</v>
+      </c>
+      <c r="D46" t="s">
+        <v>287</v>
       </c>
       <c r="E46" t="s">
-        <v>278</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>274</v>
       </c>
-      <c r="B47" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Communication</v>
-      </c>
-      <c r="C47" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>California</v>
-      </c>
-      <c r="D47" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Springfield</v>
+      <c r="B47" t="s">
+        <v>286</v>
+      </c>
+      <c r="C47" t="s">
+        <v>288</v>
+      </c>
+      <c r="D47" t="s">
+        <v>2</v>
       </c>
       <c r="E47" t="s">
-        <v>278</v>
+        <v>137</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>275</v>
       </c>
-      <c r="B48" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Engineering</v>
-      </c>
-      <c r="C48" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Missouri</v>
-      </c>
-      <c r="D48" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Las Vegas</v>
+      <c r="B48" t="s">
+        <v>289</v>
+      </c>
+      <c r="C48" t="s">
+        <v>284</v>
+      </c>
+      <c r="D48" t="s">
+        <v>2</v>
       </c>
       <c r="E48" t="s">
-        <v>278</v>
+        <v>137</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>276</v>
       </c>
-      <c r="B49" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Engineering</v>
-      </c>
-      <c r="C49" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Florida</v>
-      </c>
-      <c r="D49" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Las Vegas</v>
+      <c r="B49" t="s">
+        <v>285</v>
+      </c>
+      <c r="C49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" t="s">
+        <v>2</v>
       </c>
       <c r="E49" t="s">
-        <v>278</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>277</v>
       </c>
-      <c r="B50" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Communication</v>
-      </c>
-      <c r="C50" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Florida</v>
-      </c>
-      <c r="D50" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Springfield</v>
+      <c r="B50" t="s">
+        <v>285</v>
+      </c>
+      <c r="C50" t="s">
+        <v>284</v>
+      </c>
+      <c r="D50" t="s">
+        <v>283</v>
       </c>
       <c r="E50" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>279</v>
-      </c>
-      <c r="C51" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>California</v>
-      </c>
-      <c r="D51" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Springfield</v>
-      </c>
-      <c r="E51" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>281</v>
-      </c>
-      <c r="C52" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Missouri</v>
-      </c>
-      <c r="D52" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Las Vegas</v>
-      </c>
-      <c r="E52" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>282</v>
-      </c>
-      <c r="C53" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>California</v>
-      </c>
-      <c r="D53" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Pensacola</v>
-      </c>
-      <c r="E53" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>284</v>
-      </c>
-      <c r="C54" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Florida</v>
-      </c>
-      <c r="D54" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Springfield</v>
-      </c>
-      <c r="E54" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>285</v>
-      </c>
-      <c r="C55" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>California</v>
-      </c>
-      <c r="D55" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Las Vegas</v>
-      </c>
-      <c r="E55" t="s">
-        <v>283</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -3599,331 +3382,696 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A63"/>
+  <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="57.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Westminster College</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Lindenwood University</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Ozarks Technical Community College</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B4" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Missouri State University West Plains</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B5" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Pinnacle Career Institute North Kansas City</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B6" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Harris Stowe State University</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B7" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Lindenwood University</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B8" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Vatterott College Berkeley</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>174</v>
+      </c>
+      <c r="B9" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Fontbonne University</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B10" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Sanford Brown College St Peters</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>176</v>
+      </c>
+      <c r="B11" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Pinnacle Career Institute North Kansas City</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>177</v>
+      </c>
+      <c r="B12" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Metropolitan Community College Maple Woods</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>178</v>
+      </c>
+      <c r="B13" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Kansas City Art Institute</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>179</v>
+      </c>
+      <c r="B14" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Culver Stockton College</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>180</v>
+      </c>
+      <c r="B15" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Avila University</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>181</v>
+      </c>
+      <c r="B16" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Missouri State University West Plains</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>182</v>
+      </c>
+      <c r="B17" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Southeast Missouri Hospital College of Nursing and Health Sciences</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>183</v>
+      </c>
+      <c r="B18" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Metropolitan Community College Blue River</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>184</v>
+      </c>
+      <c r="B19" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Everest College Springfield</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>185</v>
+      </c>
+      <c r="B20" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Metro Business College Rolla</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>186</v>
+      </c>
+      <c r="B21" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>University of Missouri Columbia</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>187</v>
+      </c>
+      <c r="B22" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Metro Business College Arnold</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>188</v>
+      </c>
+      <c r="B23" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Chamberlain College of Nursing Missouri</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>189</v>
+      </c>
+      <c r="B24" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Ozarks Technical Community College</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>190</v>
+      </c>
+      <c r="B25" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>College of the Ozarks</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>191</v>
+      </c>
+      <c r="B26" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Metro Business College Jefferson City</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>192</v>
+      </c>
+      <c r="B27" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Harris Stowe State University</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>193</v>
+      </c>
+      <c r="B28" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>ITT Technical Institute Arnold</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>194</v>
+      </c>
+      <c r="B29" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>ITT Technical Institute Arnold</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>195</v>
+      </c>
+      <c r="B30" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>North Central Missouri College</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>196</v>
+      </c>
+      <c r="B31" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Park University</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>197</v>
+      </c>
+      <c r="B32" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Vatterott College Berkeley</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>198</v>
+      </c>
+      <c r="B33" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Missouri State University West Plains</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>199</v>
+      </c>
+      <c r="B34" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Southeast Missouri Hospital College of Nursing and Health Sciences</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>200</v>
+      </c>
+      <c r="B35" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>University of Missouri St Louis</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>201</v>
+      </c>
+      <c r="B36" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Webster University</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>202</v>
+      </c>
+      <c r="B37" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Central Methodist University College of Liberal Arts &amp; Sciences</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>203</v>
+      </c>
+      <c r="B38" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Cottey College</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>204</v>
+      </c>
+      <c r="B39" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Metropolitan Community College Blue River</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>205</v>
+      </c>
+      <c r="B40" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Lincoln University</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>206</v>
+      </c>
+      <c r="B41" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Columbia College</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>207</v>
+      </c>
+      <c r="B42" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Wentworth Military Academy &amp; Junior College</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>208</v>
+      </c>
+      <c r="B43" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>University of Phoenix Kansas City Campus</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>209</v>
+      </c>
+      <c r="B44" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Crowder College</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>210</v>
+      </c>
+      <c r="B45" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Columbia College</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>211</v>
+      </c>
+      <c r="B46" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Calvary Bible College and Theological Seminary</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>212</v>
+      </c>
+      <c r="B47" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Saint Louis Community College</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>213</v>
+      </c>
+      <c r="B48" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Wentworth Military Academy &amp; Junior College</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>214</v>
+      </c>
+      <c r="B49" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>University of Missouri Columbia</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>215</v>
+      </c>
+      <c r="B50" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Brown Mackie College St Louis</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>216</v>
+      </c>
+      <c r="B51" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Vatterott College Berkeley</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>217</v>
+      </c>
+      <c r="B52" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Rockhurst University</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>218</v>
+      </c>
+      <c r="B53" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Three Rivers Community College</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>219</v>
+      </c>
+      <c r="B54" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Vatterott College Saint Joseph</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>219</v>
+      </c>
+      <c r="B55" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Metropolitan Community College Business &amp; Technology</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>220</v>
+      </c>
+      <c r="B56" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Jefferson College</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>221</v>
+      </c>
+      <c r="B57" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>ITT Technical Institute Arnold</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>222</v>
+      </c>
+      <c r="B58" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Avila University</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>223</v>
+      </c>
+      <c r="B59" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Grantham University</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>224</v>
+      </c>
+      <c r="B60" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Hannibal LaGrange University</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>225</v>
+      </c>
+      <c r="B61" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Calvary Bible College and Theological Seminary</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>226</v>
+      </c>
+      <c r="B62" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Missouri Western State University</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>227</v>
+      </c>
+      <c r="B63" t="str">
+        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
+        <v>Grantham University</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>280</v>
+      </c>
+      <c r="B3" t="s">
+        <v>284</v>
+      </c>
+      <c r="C3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>281</v>
+      </c>
+      <c r="B4" t="s">
+        <v>284</v>
+      </c>
+      <c r="C4" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>282</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+      <c r="B1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>227</v>
+        <v>282</v>
+      </c>
+      <c r="B2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More test data and more queries
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="1875" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="1875"/>
   </bookViews>
   <sheets>
     <sheet name="School" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="299">
   <si>
     <t>Avila University</t>
   </si>
@@ -898,14 +898,49 @@
   </si>
   <si>
     <t>Communication</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>school</t>
+  </si>
+  <si>
+    <t>president</t>
+  </si>
+  <si>
+    <t>vicepresident</t>
+  </si>
+  <si>
+    <t>treasurer</t>
+  </si>
+  <si>
+    <t>secretary</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>major</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -933,8 +968,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1249,9 +1285,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C113"/>
+  <dimension ref="A1:C114"/>
   <sheetViews>
-    <sheetView topLeftCell="A87" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1259,21 +1295,20 @@
     <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="str">
-        <f ca="1">INDEX(A5:A12,RAND()*10+0.5)</f>
-        <v>Central Methodist University College of Liberal Arts &amp; Sciences</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -1284,10 +1319,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -1295,10 +1330,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -1306,10 +1341,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -1317,10 +1352,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -1328,10 +1363,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -1339,10 +1374,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -1350,10 +1385,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
@@ -1361,10 +1396,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
@@ -1372,10 +1407,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -1383,10 +1418,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -1394,10 +1429,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
@@ -1405,10 +1440,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
@@ -1416,10 +1451,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
@@ -1427,10 +1462,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
@@ -1438,10 +1473,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -1449,10 +1484,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
         <v>2</v>
@@ -1460,10 +1495,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
@@ -1471,10 +1506,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
@@ -1482,10 +1517,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
@@ -1493,7 +1528,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
         <v>4</v>
@@ -1504,10 +1539,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
@@ -1515,10 +1550,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B24" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="C24" t="s">
         <v>2</v>
@@ -1526,10 +1561,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>
@@ -1537,10 +1572,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
         <v>2</v>
@@ -1548,7 +1583,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B27" t="s">
         <v>38</v>
@@ -1559,10 +1594,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C28" t="s">
         <v>2</v>
@@ -1570,10 +1605,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C29" t="s">
         <v>2</v>
@@ -1581,10 +1616,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B30" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="C30" t="s">
         <v>2</v>
@@ -1592,10 +1627,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B31" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C31" t="s">
         <v>2</v>
@@ -1603,10 +1638,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B32" t="s">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="C32" t="s">
         <v>2</v>
@@ -1614,10 +1649,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B33" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="C33" t="s">
         <v>2</v>
@@ -1625,10 +1660,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="C34" t="s">
         <v>2</v>
@@ -1636,7 +1671,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B35" t="s">
         <v>38</v>
@@ -1647,10 +1682,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B36" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="C36" t="s">
         <v>2</v>
@@ -1658,10 +1693,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B37" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C37" t="s">
         <v>2</v>
@@ -1669,10 +1704,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B38" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C38" t="s">
         <v>2</v>
@@ -1680,10 +1715,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="C39" t="s">
         <v>2</v>
@@ -1691,10 +1726,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B40" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="C40" t="s">
         <v>2</v>
@@ -1702,10 +1737,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B41" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C41" t="s">
         <v>2</v>
@@ -1713,10 +1748,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B42" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="C42" t="s">
         <v>2</v>
@@ -1724,10 +1759,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B43" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="C43" t="s">
         <v>2</v>
@@ -1735,10 +1770,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B44" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="C44" t="s">
         <v>2</v>
@@ -1746,10 +1781,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B45" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C45" t="s">
         <v>2</v>
@@ -1757,10 +1792,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B46" t="s">
-        <v>1</v>
+        <v>71</v>
       </c>
       <c r="C46" t="s">
         <v>2</v>
@@ -1768,10 +1803,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B47" t="s">
-        <v>74</v>
+        <v>1</v>
       </c>
       <c r="C47" t="s">
         <v>2</v>
@@ -1779,10 +1814,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B48" t="s">
-        <v>1</v>
+        <v>74</v>
       </c>
       <c r="C48" t="s">
         <v>2</v>
@@ -1790,7 +1825,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B49" t="s">
         <v>1</v>
@@ -1801,7 +1836,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B50" t="s">
         <v>1</v>
@@ -1812,10 +1847,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B51" t="s">
-        <v>79</v>
+        <v>1</v>
       </c>
       <c r="C51" t="s">
         <v>2</v>
@@ -1823,10 +1858,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B52" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="C52" t="s">
         <v>2</v>
@@ -1834,10 +1869,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B53" t="s">
-        <v>82</v>
+        <v>38</v>
       </c>
       <c r="C53" t="s">
         <v>2</v>
@@ -1845,10 +1880,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B54" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="C54" t="s">
         <v>2</v>
@@ -1856,10 +1891,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B55" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="C55" t="s">
         <v>2</v>
@@ -1867,10 +1902,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B56" t="s">
-        <v>86</v>
+        <v>4</v>
       </c>
       <c r="C56" t="s">
         <v>2</v>
@@ -1878,10 +1913,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B57" t="s">
-        <v>58</v>
+        <v>86</v>
       </c>
       <c r="C57" t="s">
         <v>2</v>
@@ -1889,10 +1924,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B58" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C58" t="s">
         <v>2</v>
@@ -1900,10 +1935,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B59" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="C59" t="s">
         <v>2</v>
@@ -1911,10 +1946,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B60" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C60" t="s">
         <v>2</v>
@@ -1922,10 +1957,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B61" t="s">
-        <v>11</v>
+        <v>92</v>
       </c>
       <c r="C61" t="s">
         <v>2</v>
@@ -1933,10 +1968,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B62" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="C62" t="s">
         <v>2</v>
@@ -1944,10 +1979,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B63" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="C63" t="s">
         <v>2</v>
@@ -1955,10 +1990,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B64" t="s">
-        <v>1</v>
+        <v>96</v>
       </c>
       <c r="C64" t="s">
         <v>2</v>
@@ -1966,10 +2001,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B65" t="s">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="C65" t="s">
         <v>2</v>
@@ -1977,10 +2012,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B66" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C66" t="s">
         <v>2</v>
@@ -1988,10 +2023,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B67" t="s">
-        <v>63</v>
+        <v>101</v>
       </c>
       <c r="C67" t="s">
         <v>2</v>
@@ -1999,10 +2034,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B68" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="C68" t="s">
         <v>2</v>
@@ -2010,10 +2045,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B69" t="s">
-        <v>105</v>
+        <v>4</v>
       </c>
       <c r="C69" t="s">
         <v>2</v>
@@ -2021,10 +2056,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B70" t="s">
-        <v>1</v>
+        <v>105</v>
       </c>
       <c r="C70" t="s">
         <v>2</v>
@@ -2032,7 +2067,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B71" t="s">
         <v>1</v>
@@ -2043,10 +2078,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B72" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="C72" t="s">
         <v>2</v>
@@ -2054,10 +2089,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B73" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="C73" t="s">
         <v>2</v>
@@ -2065,7 +2100,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B74" t="s">
         <v>1</v>
@@ -2076,10 +2111,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B75" t="s">
-        <v>112</v>
+        <v>1</v>
       </c>
       <c r="C75" t="s">
         <v>2</v>
@@ -2087,10 +2122,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B76" t="s">
-        <v>38</v>
+        <v>112</v>
       </c>
       <c r="C76" t="s">
         <v>2</v>
@@ -2098,7 +2133,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B77" t="s">
         <v>38</v>
@@ -2109,10 +2144,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B78" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="C78" t="s">
         <v>2</v>
@@ -2120,10 +2155,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B79" t="s">
-        <v>117</v>
+        <v>6</v>
       </c>
       <c r="C79" t="s">
         <v>2</v>
@@ -2131,10 +2166,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B80" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C80" t="s">
         <v>2</v>
@@ -2142,10 +2177,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B81" t="s">
-        <v>66</v>
+        <v>119</v>
       </c>
       <c r="C81" t="s">
         <v>2</v>
@@ -2153,7 +2188,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B82" t="s">
         <v>66</v>
@@ -2164,10 +2199,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B83" t="s">
-        <v>123</v>
+        <v>66</v>
       </c>
       <c r="C83" t="s">
         <v>2</v>
@@ -2175,10 +2210,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B84" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C84" t="s">
         <v>2</v>
@@ -2186,10 +2221,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B85" t="s">
-        <v>6</v>
+        <v>125</v>
       </c>
       <c r="C85" t="s">
         <v>2</v>
@@ -2197,10 +2232,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B86" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="C86" t="s">
         <v>2</v>
@@ -2208,7 +2243,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B87" t="s">
         <v>38</v>
@@ -2219,10 +2254,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B88" t="s">
-        <v>130</v>
+        <v>38</v>
       </c>
       <c r="C88" t="s">
         <v>2</v>
@@ -2230,10 +2265,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B89" t="s">
-        <v>21</v>
+        <v>130</v>
       </c>
       <c r="C89" t="s">
         <v>2</v>
@@ -2241,10 +2276,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B90" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="C90" t="s">
         <v>2</v>
@@ -2252,10 +2287,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B91" t="s">
-        <v>134</v>
+        <v>38</v>
       </c>
       <c r="C91" t="s">
         <v>2</v>
@@ -2263,10 +2298,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B92" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C92" t="s">
         <v>2</v>
@@ -2274,10 +2309,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B93" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C93" t="s">
         <v>2</v>
@@ -2285,10 +2320,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B94" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C94" t="s">
         <v>2</v>
@@ -2296,10 +2331,10 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B95" t="s">
-        <v>21</v>
+        <v>140</v>
       </c>
       <c r="C95" t="s">
         <v>2</v>
@@ -2307,10 +2342,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B96" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C96" t="s">
         <v>2</v>
@@ -2318,10 +2353,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B97" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="C97" t="s">
         <v>2</v>
@@ -2329,10 +2364,10 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B98" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="C98" t="s">
         <v>2</v>
@@ -2340,10 +2375,10 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B99" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C99" t="s">
         <v>2</v>
@@ -2351,10 +2386,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B100" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="C100" t="s">
         <v>2</v>
@@ -2362,10 +2397,10 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B101" t="s">
-        <v>148</v>
+        <v>38</v>
       </c>
       <c r="C101" t="s">
         <v>2</v>
@@ -2373,10 +2408,10 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B102" t="s">
-        <v>63</v>
+        <v>148</v>
       </c>
       <c r="C102" t="s">
         <v>2</v>
@@ -2384,10 +2419,10 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B103" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="C103" t="s">
         <v>2</v>
@@ -2395,10 +2430,10 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B104" t="s">
-        <v>92</v>
+        <v>1</v>
       </c>
       <c r="C104" t="s">
         <v>2</v>
@@ -2406,10 +2441,10 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B105" t="s">
-        <v>4</v>
+        <v>92</v>
       </c>
       <c r="C105" t="s">
         <v>2</v>
@@ -2417,10 +2452,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B106" t="s">
-        <v>154</v>
+        <v>4</v>
       </c>
       <c r="C106" t="s">
         <v>2</v>
@@ -2428,10 +2463,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B107" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C107" t="s">
         <v>2</v>
@@ -2439,10 +2474,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B108" t="s">
-        <v>38</v>
+        <v>156</v>
       </c>
       <c r="C108" t="s">
         <v>2</v>
@@ -2450,7 +2485,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B109" t="s">
         <v>38</v>
@@ -2461,10 +2496,10 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B110" t="s">
-        <v>160</v>
+        <v>38</v>
       </c>
       <c r="C110" t="s">
         <v>2</v>
@@ -2472,10 +2507,10 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B111" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C111" t="s">
         <v>2</v>
@@ -2483,10 +2518,10 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B112" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C112" t="s">
         <v>2</v>
@@ -2494,12 +2529,23 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
+        <v>163</v>
+      </c>
+      <c r="B113" t="s">
+        <v>164</v>
+      </c>
+      <c r="C113" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>165</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B114" t="s">
         <v>162</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C114" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2510,11 +2556,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2525,26 +2569,26 @@
     <col min="5" max="5" width="62" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>228</v>
-      </c>
-      <c r="B1" t="s">
-        <v>285</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>73</v>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B2" t="s">
         <v>285</v>
@@ -2553,58 +2597,58 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>283</v>
+        <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B4" t="s">
         <v>286</v>
       </c>
       <c r="C4" t="s">
-        <v>288</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>287</v>
       </c>
       <c r="E4" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B5" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>288</v>
       </c>
       <c r="D5" t="s">
-        <v>287</v>
+        <v>2</v>
       </c>
       <c r="E5" t="s">
         <v>78</v>
@@ -2612,78 +2656,78 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B6" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="C6" t="s">
-        <v>288</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>287</v>
       </c>
       <c r="E6" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B7" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C7" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="D7" t="s">
-        <v>287</v>
+        <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>159</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B8" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="C8" t="s">
         <v>284</v>
       </c>
       <c r="D8" t="s">
-        <v>2</v>
+        <v>287</v>
       </c>
       <c r="E8" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B9" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C9" t="s">
         <v>284</v>
       </c>
       <c r="D9" t="s">
-        <v>283</v>
+        <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B10" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="C10" t="s">
         <v>284</v>
@@ -2692,114 +2736,114 @@
         <v>283</v>
       </c>
       <c r="E10" t="s">
-        <v>95</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B11" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C11" t="s">
         <v>284</v>
       </c>
       <c r="D11" t="s">
-        <v>2</v>
+        <v>283</v>
       </c>
       <c r="E11" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B12" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="C12" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D12" t="s">
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B13" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C13" t="s">
         <v>288</v>
       </c>
       <c r="D13" t="s">
-        <v>283</v>
+        <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>161</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B14" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
+        <v>288</v>
       </c>
       <c r="D14" t="s">
         <v>283</v>
       </c>
       <c r="E14" t="s">
-        <v>95</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B15" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C15" t="s">
-        <v>288</v>
+        <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E15" t="s">
-        <v>31</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B16" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
+        <v>288</v>
       </c>
       <c r="D16" t="s">
-        <v>2</v>
+        <v>287</v>
       </c>
       <c r="E16" t="s">
-        <v>108</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B17" t="s">
         <v>285</v>
@@ -2808,32 +2852,32 @@
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>287</v>
+        <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>143</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B18" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>2</v>
+        <v>287</v>
       </c>
       <c r="E18" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B19" t="s">
         <v>286</v>
@@ -2842,35 +2886,35 @@
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>283</v>
+        <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>94</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B20" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C20" t="s">
-        <v>288</v>
+        <v>4</v>
       </c>
       <c r="D20" t="s">
         <v>283</v>
       </c>
       <c r="E20" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B21" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C21" t="s">
         <v>288</v>
@@ -2879,29 +2923,29 @@
         <v>283</v>
       </c>
       <c r="E21" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B22" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C22" t="s">
-        <v>4</v>
+        <v>288</v>
       </c>
       <c r="D22" t="s">
-        <v>2</v>
+        <v>283</v>
       </c>
       <c r="E22" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B23" t="s">
         <v>289</v>
@@ -2913,80 +2957,80 @@
         <v>2</v>
       </c>
       <c r="E23" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B24" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="C24" t="s">
-        <v>284</v>
+        <v>4</v>
       </c>
       <c r="D24" t="s">
         <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B25" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C25" t="s">
         <v>284</v>
       </c>
       <c r="D25" t="s">
-        <v>283</v>
+        <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>141</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B26" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C26" t="s">
-        <v>4</v>
+        <v>284</v>
       </c>
       <c r="D26" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E26" t="s">
-        <v>111</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B27" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C27" t="s">
-        <v>288</v>
+        <v>4</v>
       </c>
       <c r="D27" t="s">
         <v>287</v>
       </c>
       <c r="E27" t="s">
-        <v>158</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B28" t="s">
         <v>289</v>
@@ -2995,15 +3039,15 @@
         <v>288</v>
       </c>
       <c r="D28" t="s">
-        <v>2</v>
+        <v>287</v>
       </c>
       <c r="E28" t="s">
-        <v>35</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B29" t="s">
         <v>289</v>
@@ -3012,327 +3056,327 @@
         <v>288</v>
       </c>
       <c r="D29" t="s">
-        <v>287</v>
+        <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B30" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="C30" t="s">
-        <v>4</v>
+        <v>288</v>
       </c>
       <c r="D30" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="E30" t="s">
-        <v>133</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B31" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C31" t="s">
-        <v>284</v>
+        <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>2</v>
+        <v>283</v>
       </c>
       <c r="E31" t="s">
-        <v>3</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B32" t="s">
         <v>286</v>
       </c>
       <c r="C32" t="s">
-        <v>4</v>
+        <v>284</v>
       </c>
       <c r="D32" t="s">
-        <v>287</v>
+        <v>2</v>
       </c>
       <c r="E32" t="s">
-        <v>62</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B33" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C33" t="s">
-        <v>288</v>
+        <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="E33" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B34" t="s">
         <v>289</v>
       </c>
       <c r="C34" t="s">
-        <v>4</v>
+        <v>288</v>
       </c>
       <c r="D34" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E34" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B35" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="C35" t="s">
-        <v>288</v>
+        <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="E35" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B36" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C36" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="D36" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E36" t="s">
-        <v>126</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B37" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C37" t="s">
         <v>284</v>
       </c>
       <c r="D37" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="E37" t="s">
-        <v>83</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B38" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="C38" t="s">
         <v>284</v>
       </c>
       <c r="D38" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E38" t="s">
-        <v>121</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B39" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C39" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D39" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="E39" t="s">
-        <v>14</v>
+        <v>121</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B40" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="C40" t="s">
-        <v>4</v>
+        <v>288</v>
       </c>
       <c r="D40" t="s">
-        <v>2</v>
+        <v>283</v>
       </c>
       <c r="E40" t="s">
-        <v>67</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B41" t="s">
         <v>286</v>
       </c>
       <c r="C41" t="s">
-        <v>288</v>
+        <v>4</v>
       </c>
       <c r="D41" t="s">
-        <v>283</v>
+        <v>2</v>
       </c>
       <c r="E41" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B42" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C42" t="s">
-        <v>4</v>
+        <v>288</v>
       </c>
       <c r="D42" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E42" t="s">
-        <v>62</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B43" t="s">
         <v>289</v>
       </c>
       <c r="C43" t="s">
-        <v>288</v>
+        <v>4</v>
       </c>
       <c r="D43" t="s">
-        <v>2</v>
+        <v>287</v>
       </c>
       <c r="E43" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B44" t="s">
         <v>289</v>
       </c>
       <c r="C44" t="s">
-        <v>4</v>
+        <v>288</v>
       </c>
       <c r="D44" t="s">
         <v>2</v>
       </c>
       <c r="E44" t="s">
-        <v>110</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B45" t="s">
         <v>289</v>
       </c>
       <c r="C45" t="s">
-        <v>284</v>
+        <v>4</v>
       </c>
       <c r="D45" t="s">
-        <v>283</v>
+        <v>2</v>
       </c>
       <c r="E45" t="s">
-        <v>22</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B46" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="C46" t="s">
         <v>284</v>
       </c>
       <c r="D46" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E46" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B47" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C47" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D47" t="s">
-        <v>2</v>
+        <v>287</v>
       </c>
       <c r="E47" t="s">
-        <v>137</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B48" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C48" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="D48" t="s">
         <v>2</v>
@@ -3343,632 +3387,789 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B49" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="C49" t="s">
-        <v>4</v>
+        <v>284</v>
       </c>
       <c r="D49" t="s">
         <v>2</v>
       </c>
       <c r="E49" t="s">
-        <v>61</v>
+        <v>137</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B50" t="s">
         <v>285</v>
       </c>
       <c r="C50" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" t="s">
+        <v>2</v>
+      </c>
+      <c r="E50" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>277</v>
+      </c>
+      <c r="B51" t="s">
+        <v>285</v>
+      </c>
+      <c r="C51" t="s">
         <v>284</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D51" t="s">
         <v>283</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E51" t="s">
         <v>131</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B63"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.28515625" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" customWidth="1"/>
+    <col min="3" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>166</v>
       </c>
-      <c r="B1" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Westminster College</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E2" t="s">
+        <v>230</v>
+      </c>
+      <c r="F2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>167</v>
       </c>
-      <c r="B2" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Lindenwood University</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D3" t="s">
+        <v>230</v>
+      </c>
+      <c r="E3" t="s">
+        <v>231</v>
+      </c>
+      <c r="F3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>168</v>
       </c>
-      <c r="B3" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Ozarks Technical Community College</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" t="s">
+        <v>230</v>
+      </c>
+      <c r="D4" t="s">
+        <v>231</v>
+      </c>
+      <c r="E4" t="s">
+        <v>232</v>
+      </c>
+      <c r="F4" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>169</v>
       </c>
-      <c r="B4" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Missouri State University West Plains</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" t="s">
+        <v>231</v>
+      </c>
+      <c r="D5" t="s">
+        <v>232</v>
+      </c>
+      <c r="E5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>170</v>
       </c>
-      <c r="B5" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Pinnacle Career Institute North Kansas City</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
+        <v>232</v>
+      </c>
+      <c r="D6" t="s">
+        <v>233</v>
+      </c>
+      <c r="E6" t="s">
+        <v>234</v>
+      </c>
+      <c r="F6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>171</v>
       </c>
-      <c r="B6" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Harris Stowe State University</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>172</v>
       </c>
-      <c r="B7" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Lindenwood University</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>173</v>
       </c>
-      <c r="B8" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Vatterott College Berkeley</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>174</v>
       </c>
-      <c r="B9" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Fontbonne University</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>175</v>
       </c>
-      <c r="B10" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Sanford Brown College St Peters</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C11" t="s">
+        <v>228</v>
+      </c>
+      <c r="D11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E11" t="s">
+        <v>230</v>
+      </c>
+      <c r="F11" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>176</v>
       </c>
-      <c r="B11" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Pinnacle Career Institute North Kansas City</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>229</v>
+      </c>
+      <c r="D12" t="s">
+        <v>230</v>
+      </c>
+      <c r="E12" t="s">
+        <v>231</v>
+      </c>
+      <c r="F12" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>177</v>
       </c>
-      <c r="B12" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Metropolitan Community College Maple Woods</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" t="s">
+        <v>230</v>
+      </c>
+      <c r="D13" t="s">
+        <v>231</v>
+      </c>
+      <c r="E13" t="s">
+        <v>232</v>
+      </c>
+      <c r="F13" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>178</v>
       </c>
-      <c r="B13" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Kansas City Art Institute</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" t="s">
+        <v>231</v>
+      </c>
+      <c r="D14" t="s">
+        <v>232</v>
+      </c>
+      <c r="E14" t="s">
+        <v>233</v>
+      </c>
+      <c r="F14" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>179</v>
       </c>
-      <c r="B14" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Culver Stockton College</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
+        <v>142</v>
+      </c>
+      <c r="C15" t="s">
+        <v>232</v>
+      </c>
+      <c r="D15" t="s">
+        <v>233</v>
+      </c>
+      <c r="E15" t="s">
+        <v>234</v>
+      </c>
+      <c r="F15" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>180</v>
       </c>
-      <c r="B15" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Avila University</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>181</v>
       </c>
-      <c r="B16" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Missouri State University West Plains</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>182</v>
       </c>
-      <c r="B17" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Southeast Missouri Hospital College of Nursing and Health Sciences</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>183</v>
       </c>
-      <c r="B18" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Metropolitan Community College Blue River</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
+        <v>142</v>
+      </c>
+      <c r="C19" t="s">
+        <v>228</v>
+      </c>
+      <c r="D19" t="s">
+        <v>229</v>
+      </c>
+      <c r="E19" t="s">
+        <v>230</v>
+      </c>
+      <c r="F19" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>184</v>
       </c>
-      <c r="B19" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Everest College Springfield</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
+        <v>145</v>
+      </c>
+      <c r="C20" t="s">
+        <v>229</v>
+      </c>
+      <c r="D20" t="s">
+        <v>230</v>
+      </c>
+      <c r="E20" t="s">
+        <v>231</v>
+      </c>
+      <c r="F20" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>185</v>
       </c>
-      <c r="B20" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Metro Business College Rolla</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>230</v>
+      </c>
+      <c r="D21" t="s">
+        <v>231</v>
+      </c>
+      <c r="E21" t="s">
+        <v>232</v>
+      </c>
+      <c r="F21" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>186</v>
       </c>
-      <c r="B21" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>University of Missouri Columbia</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" t="s">
+        <v>231</v>
+      </c>
+      <c r="D22" t="s">
+        <v>232</v>
+      </c>
+      <c r="E22" t="s">
+        <v>233</v>
+      </c>
+      <c r="F22" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>187</v>
       </c>
-      <c r="B22" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Metro Business College Arnold</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B23" t="s">
+        <v>127</v>
+      </c>
+      <c r="C23" t="s">
+        <v>232</v>
+      </c>
+      <c r="D23" t="s">
+        <v>233</v>
+      </c>
+      <c r="E23" t="s">
+        <v>234</v>
+      </c>
+      <c r="F23" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>188</v>
       </c>
-      <c r="B23" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Chamberlain College of Nursing Missouri</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>189</v>
       </c>
-      <c r="B24" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Ozarks Technical Community College</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>190</v>
       </c>
-      <c r="B25" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>College of the Ozarks</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>191</v>
       </c>
-      <c r="B26" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Metro Business College Jefferson City</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B27" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>192</v>
       </c>
-      <c r="B27" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Harris Stowe State University</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>193</v>
       </c>
-      <c r="B28" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>ITT Technical Institute Arnold</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>194</v>
       </c>
-      <c r="B29" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>ITT Technical Institute Arnold</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>195</v>
       </c>
-      <c r="B30" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>North Central Missouri College</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B31" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>196</v>
       </c>
-      <c r="B31" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Park University</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>197</v>
-      </c>
-      <c r="B32" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Vatterott College Berkeley</v>
+      <c r="B32" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>198</v>
-      </c>
-      <c r="B33" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Missouri State University West Plains</v>
+        <v>197</v>
+      </c>
+      <c r="B33" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>199</v>
-      </c>
-      <c r="B34" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Southeast Missouri Hospital College of Nursing and Health Sciences</v>
+        <v>198</v>
+      </c>
+      <c r="B34" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>200</v>
-      </c>
-      <c r="B35" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>University of Missouri St Louis</v>
+        <v>199</v>
+      </c>
+      <c r="B35" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>201</v>
-      </c>
-      <c r="B36" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Webster University</v>
+        <v>200</v>
+      </c>
+      <c r="B36" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>202</v>
-      </c>
-      <c r="B37" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Central Methodist University College of Liberal Arts &amp; Sciences</v>
+        <v>201</v>
+      </c>
+      <c r="B37" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>203</v>
-      </c>
-      <c r="B38" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Cottey College</v>
+        <v>202</v>
+      </c>
+      <c r="B38" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>204</v>
-      </c>
-      <c r="B39" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Metropolitan Community College Blue River</v>
+        <v>203</v>
+      </c>
+      <c r="B39" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>205</v>
-      </c>
-      <c r="B40" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Lincoln University</v>
+        <v>204</v>
+      </c>
+      <c r="B40" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>206</v>
-      </c>
-      <c r="B41" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Columbia College</v>
+        <v>205</v>
+      </c>
+      <c r="B41" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>207</v>
-      </c>
-      <c r="B42" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Wentworth Military Academy &amp; Junior College</v>
+        <v>206</v>
+      </c>
+      <c r="B42" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>208</v>
-      </c>
-      <c r="B43" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>University of Phoenix Kansas City Campus</v>
+        <v>207</v>
+      </c>
+      <c r="B43" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>209</v>
-      </c>
-      <c r="B44" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Crowder College</v>
+        <v>208</v>
+      </c>
+      <c r="B44" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>210</v>
-      </c>
-      <c r="B45" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Columbia College</v>
+        <v>209</v>
+      </c>
+      <c r="B45" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>211</v>
-      </c>
-      <c r="B46" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Calvary Bible College and Theological Seminary</v>
+        <v>210</v>
+      </c>
+      <c r="B46" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>212</v>
-      </c>
-      <c r="B47" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Saint Louis Community College</v>
+        <v>211</v>
+      </c>
+      <c r="B47" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>213</v>
-      </c>
-      <c r="B48" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Wentworth Military Academy &amp; Junior College</v>
+        <v>212</v>
+      </c>
+      <c r="B48" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>214</v>
-      </c>
-      <c r="B49" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>University of Missouri Columbia</v>
+        <v>213</v>
+      </c>
+      <c r="B49" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>215</v>
-      </c>
-      <c r="B50" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Brown Mackie College St Louis</v>
+        <v>214</v>
+      </c>
+      <c r="B50" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>216</v>
-      </c>
-      <c r="B51" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Vatterott College Berkeley</v>
+        <v>215</v>
+      </c>
+      <c r="B51" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>217</v>
-      </c>
-      <c r="B52" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Rockhurst University</v>
+        <v>216</v>
+      </c>
+      <c r="B52" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>218</v>
-      </c>
-      <c r="B53" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Three Rivers Community College</v>
+        <v>217</v>
+      </c>
+      <c r="B53" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>219</v>
-      </c>
-      <c r="B54" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Vatterott College Saint Joseph</v>
+        <v>218</v>
+      </c>
+      <c r="B54" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>219</v>
       </c>
-      <c r="B55" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Metropolitan Community College Business &amp; Technology</v>
+      <c r="B55" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>220</v>
-      </c>
-      <c r="B56" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Jefferson College</v>
+        <v>219</v>
+      </c>
+      <c r="B56" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>221</v>
-      </c>
-      <c r="B57" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>ITT Technical Institute Arnold</v>
+        <v>220</v>
+      </c>
+      <c r="B57" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>222</v>
-      </c>
-      <c r="B58" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Avila University</v>
+        <v>221</v>
+      </c>
+      <c r="B58" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>223</v>
-      </c>
-      <c r="B59" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Grantham University</v>
+        <v>222</v>
+      </c>
+      <c r="B59" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>224</v>
-      </c>
-      <c r="B60" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Hannibal LaGrange University</v>
+        <v>223</v>
+      </c>
+      <c r="B60" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>225</v>
-      </c>
-      <c r="B61" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Calvary Bible College and Theological Seminary</v>
+        <v>224</v>
+      </c>
+      <c r="B61" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>226</v>
-      </c>
-      <c r="B62" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Missouri Western State University</v>
+        <v>225</v>
+      </c>
+      <c r="B62" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>226</v>
+      </c>
+      <c r="B63" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>227</v>
       </c>
-      <c r="B63" t="str">
-        <f ca="1">INDEX(School!$A$1:$A$113,RAND()*113+0.5)</f>
-        <v>Grantham University</v>
+      <c r="B64" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3977,20 +4178,20 @@
     <col min="3" max="3" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>278</v>
-      </c>
-      <c r="B1" t="s">
-        <v>284</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B2" t="s">
         <v>284</v>
@@ -4001,34 +4202,45 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B3" t="s">
         <v>284</v>
       </c>
       <c r="C3" t="s">
-        <v>283</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B4" t="s">
         <v>284</v>
       </c>
       <c r="C4" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>281</v>
+      </c>
+      <c r="B5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C5" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>282</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>283</v>
       </c>
     </row>
@@ -4039,11 +4251,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4052,25 +4262,36 @@
     <col min="3" max="3" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>281</v>
-      </c>
-      <c r="B1" t="s">
-        <v>284</v>
-      </c>
-      <c r="C1" t="s">
-        <v>283</v>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B2" t="s">
         <v>284</v>
       </c>
       <c r="C2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>282</v>
+      </c>
+      <c r="B3" t="s">
+        <v>284</v>
+      </c>
+      <c r="C3" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Exploring the options with Pyramid
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="1875" tabRatio="709" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="1875" tabRatio="709" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="School" sheetId="2" r:id="rId1"/>
@@ -3241,7 +3241,7 @@
       </c>
       <c r="G2">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="H2" s="9">
         <v>3</v>
@@ -3270,7 +3270,7 @@
       </c>
       <c r="G3">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="H3" s="9">
         <v>4</v>
@@ -3299,7 +3299,7 @@
       </c>
       <c r="G4">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="H4" s="9">
         <v>5</v>
@@ -3328,7 +3328,7 @@
       </c>
       <c r="G5">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H5" s="9">
         <v>6</v>
@@ -3357,7 +3357,7 @@
       </c>
       <c r="G6">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="H6" s="9">
         <v>7</v>
@@ -3386,7 +3386,7 @@
       </c>
       <c r="G7">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="H7" s="9">
         <v>8</v>
@@ -3415,7 +3415,7 @@
       </c>
       <c r="G8">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="H8" s="9">
         <v>9</v>
@@ -3444,7 +3444,7 @@
       </c>
       <c r="G9">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="H9" s="9">
         <v>10</v>
@@ -3473,7 +3473,7 @@
       </c>
       <c r="G10">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="H10" s="9">
         <v>11</v>
@@ -3502,7 +3502,7 @@
       </c>
       <c r="G11">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="H11" s="9">
         <v>12</v>
@@ -3531,7 +3531,7 @@
       </c>
       <c r="G12">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="H12" s="9">
         <v>13</v>
@@ -3560,7 +3560,7 @@
       </c>
       <c r="G13">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="H13" s="9">
         <v>14</v>
@@ -3589,7 +3589,7 @@
       </c>
       <c r="G14">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="H14" s="9">
         <v>15</v>
@@ -3618,7 +3618,7 @@
       </c>
       <c r="G15">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="H15" s="9">
         <v>16</v>
@@ -3647,7 +3647,7 @@
       </c>
       <c r="G16">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>43</v>
+        <v>109</v>
       </c>
       <c r="H16" s="9">
         <v>17</v>
@@ -3676,7 +3676,7 @@
       </c>
       <c r="G17">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="H17" s="9">
         <v>18</v>
@@ -3705,7 +3705,7 @@
       </c>
       <c r="G18">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="H18" s="9">
         <v>19</v>
@@ -3734,7 +3734,7 @@
       </c>
       <c r="G19">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="H19" s="9">
         <v>20</v>
@@ -3763,7 +3763,7 @@
       </c>
       <c r="G20">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="H20" s="9">
         <v>21</v>
@@ -3792,7 +3792,7 @@
       </c>
       <c r="G21">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>30</v>
+        <v>95</v>
       </c>
       <c r="H21" s="9">
         <v>22</v>
@@ -3821,7 +3821,7 @@
       </c>
       <c r="G22">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="H22" s="9">
         <v>23</v>
@@ -3850,7 +3850,7 @@
       </c>
       <c r="G23">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="H23" s="9">
         <v>24</v>
@@ -3879,7 +3879,7 @@
       </c>
       <c r="G24">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>86</v>
+        <v>32</v>
       </c>
       <c r="H24" s="9">
         <v>25</v>
@@ -3908,7 +3908,7 @@
       </c>
       <c r="G25">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>69</v>
+        <v>97</v>
       </c>
       <c r="H25" s="9">
         <v>26</v>
@@ -3937,7 +3937,7 @@
       </c>
       <c r="G26">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>86</v>
+        <v>18</v>
       </c>
       <c r="H26" s="9">
         <v>27</v>
@@ -3966,7 +3966,7 @@
       </c>
       <c r="G27">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>6</v>
+        <v>70</v>
       </c>
       <c r="H27" s="9">
         <v>28</v>
@@ -3995,7 +3995,7 @@
       </c>
       <c r="G28">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="H28" s="9">
         <v>29</v>
@@ -4024,7 +4024,7 @@
       </c>
       <c r="G29">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>109</v>
+        <v>38</v>
       </c>
       <c r="H29" s="9">
         <v>30</v>
@@ -4053,7 +4053,7 @@
       </c>
       <c r="G30">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="H30" s="9">
         <v>31</v>
@@ -4082,7 +4082,7 @@
       </c>
       <c r="G31">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H31" s="9">
         <v>32</v>
@@ -4111,7 +4111,7 @@
       </c>
       <c r="G32">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H32" s="9">
         <v>33</v>
@@ -4140,7 +4140,7 @@
       </c>
       <c r="G33">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="H33" s="9">
         <v>34</v>
@@ -4169,7 +4169,7 @@
       </c>
       <c r="G34">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="H34" s="9">
         <v>35</v>
@@ -4198,7 +4198,7 @@
       </c>
       <c r="G35">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>72</v>
+        <v>21</v>
       </c>
       <c r="H35" s="9">
         <v>36</v>
@@ -4227,7 +4227,7 @@
       </c>
       <c r="G36">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="H36" s="9">
         <v>37</v>
@@ -4256,7 +4256,7 @@
       </c>
       <c r="G37">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="H37" s="9">
         <v>38</v>
@@ -4285,7 +4285,7 @@
       </c>
       <c r="G38">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="H38" s="9">
         <v>39</v>
@@ -4314,7 +4314,7 @@
       </c>
       <c r="G39">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="H39" s="9">
         <v>40</v>
@@ -4372,7 +4372,7 @@
       </c>
       <c r="G41">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="H41" s="9">
         <v>42</v>
@@ -4401,7 +4401,7 @@
       </c>
       <c r="G42">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="H42" s="9">
         <v>43</v>
@@ -4430,7 +4430,7 @@
       </c>
       <c r="G43">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="H43" s="9">
         <v>44</v>
@@ -4459,7 +4459,7 @@
       </c>
       <c r="G44">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>101</v>
+        <v>66</v>
       </c>
       <c r="H44" s="9">
         <v>45</v>
@@ -4488,7 +4488,7 @@
       </c>
       <c r="G45">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="H45" s="9">
         <v>46</v>
@@ -4517,7 +4517,7 @@
       </c>
       <c r="G46">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>44</v>
+        <v>111</v>
       </c>
       <c r="H46" s="9">
         <v>47</v>
@@ -4546,7 +4546,7 @@
       </c>
       <c r="G47">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>33</v>
+        <v>79</v>
       </c>
       <c r="H47" s="9">
         <v>48</v>
@@ -4575,7 +4575,7 @@
       </c>
       <c r="G48">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="H48" s="9">
         <v>49</v>
@@ -4604,7 +4604,7 @@
       </c>
       <c r="G49">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="H49" s="9">
         <v>50</v>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="G50">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>26</v>
+        <v>93</v>
       </c>
       <c r="H50" s="9">
         <v>51</v>
@@ -4662,7 +4662,7 @@
       </c>
       <c r="G51">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="H51" s="9">
         <v>52</v>
@@ -4723,27 +4723,27 @@
       </c>
       <c r="B2">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>74</v>
+        <v>110</v>
       </c>
       <c r="C2">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="F2">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G2" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>8 52 39 48 9</v>
+        <v>48 51 37 21 52</v>
       </c>
       <c r="H2" s="9">
         <v>1</v>
@@ -4755,27 +4755,27 @@
       </c>
       <c r="B3">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E3">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F3">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G3" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>32 50 22 20 3</v>
+        <v>43 51 37 52 17</v>
       </c>
       <c r="H3" s="9">
         <v>2</v>
@@ -4787,27 +4787,27 @@
       </c>
       <c r="B4">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C4">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="D4">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="E4">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="F4">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="G4" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>23 16 16 6 36</v>
+        <v>20 48 4 7 12</v>
       </c>
       <c r="H4" s="9">
         <v>3</v>
@@ -4819,27 +4819,27 @@
       </c>
       <c r="B5">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>101</v>
+        <v>40</v>
       </c>
       <c r="C5">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="E5">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="F5">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="G5" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>7 34 12 49 17</v>
+        <v>44 46 20 14 9</v>
       </c>
       <c r="H5" s="9">
         <v>4</v>
@@ -4851,27 +4851,27 @@
       </c>
       <c r="B6">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="C6">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E6">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F6">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="G6" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>44 19 50 38 20</v>
+        <v>46 6 47 14 28</v>
       </c>
       <c r="H6" s="9">
         <v>5</v>
@@ -4883,27 +4883,27 @@
       </c>
       <c r="B7">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="C7">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D7">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="E7">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
+        <v>24</v>
+      </c>
+      <c r="F7">
+        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
         <v>40</v>
-      </c>
-      <c r="F7">
-        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>45</v>
       </c>
       <c r="G7" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>26 45 34 4 22</v>
+        <v>48 49 35 10 46</v>
       </c>
       <c r="H7" s="9">
         <v>6</v>
@@ -4915,27 +4915,27 @@
       </c>
       <c r="B8">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="D8">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="E8">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F8">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="G8" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>45 36 52 19 26</v>
+        <v>23 35 10 30 25</v>
       </c>
       <c r="H8" s="9">
         <v>7</v>
@@ -4947,27 +4947,27 @@
       </c>
       <c r="B9">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>25</v>
+        <v>108</v>
       </c>
       <c r="C9">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D9">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
+        <v>36</v>
+      </c>
+      <c r="E9">
+        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
+        <v>28</v>
+      </c>
+      <c r="F9">
+        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
         <v>26</v>
-      </c>
-      <c r="E9">
-        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>7</v>
-      </c>
-      <c r="F9">
-        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>34</v>
       </c>
       <c r="G9" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>50 39 51 23 50</v>
+        <v>30 36 11 6 19</v>
       </c>
       <c r="H9" s="9">
         <v>8</v>
@@ -4979,27 +4979,27 @@
       </c>
       <c r="B10">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="C10">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D10">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="E10">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F10">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="G10" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>20 5 3 31 26</v>
+        <v>13 51 37 9 10</v>
       </c>
       <c r="H10" s="9">
         <v>9</v>
@@ -5011,27 +5011,27 @@
       </c>
       <c r="B11">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="C11">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="D11">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="E11">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="F11">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="G11" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>51 41 43 10 51</v>
+        <v>38 49 30 34 13</v>
       </c>
       <c r="H11" s="9">
         <v>10</v>
@@ -5043,27 +5043,27 @@
       </c>
       <c r="B12">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C12">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="D12">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E12">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="F12">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="G12" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>5 42 45 4 9</v>
+        <v>40 35 43 44 8</v>
       </c>
       <c r="H12" s="9">
         <v>11</v>
@@ -5075,27 +5075,27 @@
       </c>
       <c r="B13">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="C13">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="D13">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="E13">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="F13">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G13" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>42 48 38 18 11</v>
+        <v>18 45 7 19 18</v>
       </c>
       <c r="H13" s="9">
         <v>12</v>
@@ -5107,27 +5107,27 @@
       </c>
       <c r="B14">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C14">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D14">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="E14">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="F14">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G14" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>6 5 16 47 3</v>
+        <v>40 38 25 7 50</v>
       </c>
       <c r="H14" s="9">
         <v>13</v>
@@ -5139,27 +5139,27 @@
       </c>
       <c r="B15">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>65</v>
+        <v>102</v>
       </c>
       <c r="C15">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="D15">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E15">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="F15">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="G15" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>30 29 40 10 6</v>
+        <v>32 17 48 5 23</v>
       </c>
       <c r="H15" s="9">
         <v>14</v>
@@ -5171,15 +5171,15 @@
       </c>
       <c r="B16">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>36</v>
+        <v>97</v>
       </c>
       <c r="C16">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="D16">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E16">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
@@ -5187,11 +5187,11 @@
       </c>
       <c r="F16">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="G16" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>49 10 7 28 33</v>
+        <v>21 17 28 9 31</v>
       </c>
       <c r="H16" s="9">
         <v>15</v>
@@ -5203,27 +5203,27 @@
       </c>
       <c r="B17">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C17">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D17">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E17">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="F17">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="G17" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>11 42 9 40 30</v>
+        <v>9 14 40 46 3</v>
       </c>
       <c r="H17" s="9">
         <v>16</v>
@@ -5235,27 +5235,27 @@
       </c>
       <c r="B18">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="C18">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="D18">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="E18">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="F18">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="G18" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>48 46 26 42 27</v>
+        <v>6 41 13 25 36</v>
       </c>
       <c r="H18" s="9">
         <v>17</v>
@@ -5267,27 +5267,27 @@
       </c>
       <c r="B19">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="C19">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="D19">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E19">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="F19">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="G19" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>28 37 24 50 30</v>
+        <v>21 47 19 40 23</v>
       </c>
       <c r="H19" s="9">
         <v>18</v>
@@ -5299,27 +5299,27 @@
       </c>
       <c r="B20">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>16</v>
+        <v>105</v>
       </c>
       <c r="C20">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="D20">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="E20">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F20">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="G20" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>32 28 7 21 16</v>
+        <v>8 35 46 51 44</v>
       </c>
       <c r="H20" s="9">
         <v>19</v>
@@ -5331,27 +5331,27 @@
       </c>
       <c r="B21">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="C21">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D21">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="E21">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="F21">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="G21" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>9 43 44 51 50</v>
+        <v>18 35 36 18 48</v>
       </c>
       <c r="H21" s="9">
         <v>20</v>
@@ -5363,27 +5363,27 @@
       </c>
       <c r="B22">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C22">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="D22">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E22">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="F22">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G22" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>49 25 19 23 29</v>
+        <v>19 10 17 46 10</v>
       </c>
       <c r="H22" s="9">
         <v>21</v>
@@ -5395,27 +5395,27 @@
       </c>
       <c r="B23">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C23">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="D23">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="E23">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
+        <v>13</v>
+      </c>
+      <c r="F23">
+        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
         <v>4</v>
-      </c>
-      <c r="F23">
-        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>14</v>
       </c>
       <c r="G23" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>30 51 3 52 13</v>
+        <v>29 52 18 21 6</v>
       </c>
       <c r="H23" s="9">
         <v>22</v>
@@ -5427,11 +5427,11 @@
       </c>
       <c r="B24">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>14</v>
+        <v>108</v>
       </c>
       <c r="G24" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>38 46 47 52 30</v>
+        <v>12 41 10 52 37</v>
       </c>
       <c r="H24" s="9">
         <v>23</v>
@@ -5443,11 +5443,11 @@
       </c>
       <c r="B25">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>105</v>
+        <v>67</v>
       </c>
       <c r="G25" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>41 11 48 43 51</v>
+        <v>7 26 5 23 49</v>
       </c>
       <c r="H25" s="9">
         <v>24</v>
@@ -5459,11 +5459,11 @@
       </c>
       <c r="B26">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>112</v>
+        <v>50</v>
       </c>
       <c r="G26" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>23 17 5 6 49</v>
+        <v>44 51 35 44 39</v>
       </c>
       <c r="H26" s="9">
         <v>25</v>
@@ -5475,11 +5475,11 @@
       </c>
       <c r="B27">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="G27" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>44 47 30 26 48</v>
+        <v>45 50 29 24 3</v>
       </c>
       <c r="H27" s="9">
         <v>26</v>
@@ -5491,11 +5491,11 @@
       </c>
       <c r="B28">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>28</v>
+        <v>88</v>
       </c>
       <c r="G28" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>47 4 21 46 41</v>
+        <v>24 7 23 23 31</v>
       </c>
       <c r="H28" s="9">
         <v>27</v>
@@ -5507,11 +5507,11 @@
       </c>
       <c r="B29">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G29" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>11 49 22 13 52</v>
+        <v>49 25 33 23 7</v>
       </c>
       <c r="H29" s="9">
         <v>28</v>
@@ -5523,11 +5523,11 @@
       </c>
       <c r="B30">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G30" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>44 26 34 26 39</v>
+        <v>21 48 7 39 29</v>
       </c>
       <c r="H30" s="9">
         <v>29</v>
@@ -5539,11 +5539,11 @@
       </c>
       <c r="B31">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="G31" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>9 38 52 48 12</v>
+        <v>51 39 22 39 34</v>
       </c>
       <c r="H31" s="9">
         <v>30</v>
@@ -5555,11 +5555,11 @@
       </c>
       <c r="B32">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="G32" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>44 20 30 46 5</v>
+        <v>43 24 3 7 28</v>
       </c>
       <c r="H32" s="9">
         <v>31</v>
@@ -5571,11 +5571,11 @@
       </c>
       <c r="B33">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G33" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>35 29 43 37 12</v>
+        <v>36 20 17 9 28</v>
       </c>
       <c r="H33" s="9">
         <v>32</v>
@@ -5587,11 +5587,11 @@
       </c>
       <c r="B34">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="G34" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>46 43 8 35 32</v>
+        <v>7 45 23 34 11</v>
       </c>
       <c r="H34" s="9">
         <v>33</v>
@@ -5603,11 +5603,11 @@
       </c>
       <c r="B35">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="G35" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>13 29 12 50 47</v>
+        <v>23 7 7 27 23</v>
       </c>
       <c r="H35" s="9">
         <v>34</v>
@@ -5619,11 +5619,11 @@
       </c>
       <c r="B36">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>103</v>
+        <v>29</v>
       </c>
       <c r="G36" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>37 18 6 51 28</v>
+        <v>11 37 14 43 44</v>
       </c>
       <c r="H36" s="9">
         <v>35</v>
@@ -5635,11 +5635,11 @@
       </c>
       <c r="B37">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="G37" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>33 14 45 26 6</v>
+        <v>21 13 11 38 4</v>
       </c>
       <c r="H37" s="9">
         <v>36</v>
@@ -5651,11 +5651,11 @@
       </c>
       <c r="B38">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="G38" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>34 3 49 28 13</v>
+        <v>46 4 21 50 44</v>
       </c>
       <c r="H38" s="9">
         <v>37</v>
@@ -5667,11 +5667,11 @@
       </c>
       <c r="B39">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="G39" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>49 46 36 9 38</v>
+        <v>28 36 51 37 39</v>
       </c>
       <c r="H39" s="9">
         <v>38</v>
@@ -5683,11 +5683,11 @@
       </c>
       <c r="B40">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="G40" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>34 18 34 35 6</v>
+        <v>27 49 15 18 20</v>
       </c>
       <c r="H40" s="9">
         <v>39</v>
@@ -5699,11 +5699,11 @@
       </c>
       <c r="B41">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>78</v>
+        <v>10</v>
       </c>
       <c r="G41" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>49 34 41 38 3</v>
+        <v>12 19 23 7 37</v>
       </c>
       <c r="H41" s="9">
         <v>40</v>
@@ -5715,11 +5715,11 @@
       </c>
       <c r="B42">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="G42" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>18 27 21 21 12</v>
+        <v>32 31 6 12 18</v>
       </c>
       <c r="H42" s="9">
         <v>41</v>
@@ -5731,11 +5731,11 @@
       </c>
       <c r="B43">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="G43" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>4 38 26 49 31</v>
+        <v>34 11 37 23 15</v>
       </c>
       <c r="H43" s="9">
         <v>42</v>
@@ -5747,11 +5747,11 @@
       </c>
       <c r="B44">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="G44" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>43 11 42 32 39</v>
+        <v>23 8 8 18 29</v>
       </c>
       <c r="H44" s="9">
         <v>43</v>
@@ -5763,11 +5763,11 @@
       </c>
       <c r="B45">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="G45" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>4 8 28 43 38</v>
+        <v>21 42 44 37 13</v>
       </c>
       <c r="H45" s="9">
         <v>44</v>
@@ -5779,11 +5779,11 @@
       </c>
       <c r="B46">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="G46" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>27 39 40 12 40</v>
+        <v>15 46 46 10 20</v>
       </c>
       <c r="H46" s="9">
         <v>45</v>
@@ -5795,11 +5795,11 @@
       </c>
       <c r="B47">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>98</v>
+        <v>46</v>
       </c>
       <c r="G47" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>17 15 41 18 22</v>
+        <v>40 35 18 8 5</v>
       </c>
       <c r="H47" s="9">
         <v>46</v>
@@ -5811,11 +5811,11 @@
       </c>
       <c r="B48">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>97</v>
+        <v>39</v>
       </c>
       <c r="G48" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>26 45 12 49 39</v>
+        <v>19 50 48 14 35</v>
       </c>
       <c r="H48" s="9">
         <v>47</v>
@@ -5827,11 +5827,11 @@
       </c>
       <c r="B49">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="G49" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>39 35 50 8 4</v>
+        <v>19 17 14 29 20</v>
       </c>
       <c r="H49" s="9">
         <v>48</v>
@@ -5843,11 +5843,11 @@
       </c>
       <c r="B50">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="G50" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>13 40 41 16 38</v>
+        <v>38 24 7 30 50</v>
       </c>
       <c r="H50" s="9">
         <v>49</v>
@@ -5859,11 +5859,11 @@
       </c>
       <c r="B51">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>105</v>
+        <v>66</v>
       </c>
       <c r="G51" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>44 48 42 40 47</v>
+        <v>4 52 23 42 15</v>
       </c>
       <c r="H51" s="9">
         <v>50</v>
@@ -5875,11 +5875,11 @@
       </c>
       <c r="B52">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>64</v>
+        <v>21</v>
       </c>
       <c r="G52" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>35 33 52 3 24</v>
+        <v>44 44 11 36 32</v>
       </c>
       <c r="H52" s="9">
         <v>51</v>
@@ -5891,11 +5891,11 @@
       </c>
       <c r="B53">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="G53" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>44 27 7 6 31</v>
+        <v>13 34 49 46 21</v>
       </c>
       <c r="H53" s="9">
         <v>52</v>
@@ -5907,11 +5907,11 @@
       </c>
       <c r="B54">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>17</v>
+        <v>75</v>
       </c>
       <c r="G54" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>4 21 50 29 15</v>
+        <v>4 15 41 40 35</v>
       </c>
       <c r="H54" s="9">
         <v>53</v>
@@ -5923,11 +5923,11 @@
       </c>
       <c r="B55">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="G55" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>13 46 5 35 47</v>
+        <v>37 52 20 29 10</v>
       </c>
       <c r="H55" s="9">
         <v>54</v>
@@ -5939,11 +5939,11 @@
       </c>
       <c r="B56">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>80</v>
+        <v>21</v>
       </c>
       <c r="G56" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>42 25 3 45 31</v>
+        <v>28 51 8 34 17</v>
       </c>
       <c r="H56" s="9">
         <v>55</v>
@@ -5955,11 +5955,11 @@
       </c>
       <c r="B57">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>32</v>
+        <v>80</v>
       </c>
       <c r="G57" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>14 47 33 51 45</v>
+        <v>32 38 11 49 43</v>
       </c>
       <c r="H57" s="9">
         <v>56</v>
@@ -5971,11 +5971,11 @@
       </c>
       <c r="B58">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="G58" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>3 40 50 16 22</v>
+        <v>7 44 26 36 9</v>
       </c>
       <c r="H58" s="9">
         <v>57</v>
@@ -5987,7 +5987,7 @@
       </c>
       <c r="B59">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="H59" s="9">
         <v>58</v>
@@ -5999,7 +5999,7 @@
       </c>
       <c r="B60">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>94</v>
+        <v>42</v>
       </c>
       <c r="H60" s="9">
         <v>59</v>
@@ -6011,7 +6011,7 @@
       </c>
       <c r="B61">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="H61" s="9">
         <v>60</v>
@@ -6023,7 +6023,7 @@
       </c>
       <c r="B62">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H62" s="9">
         <v>61</v>
@@ -6035,7 +6035,7 @@
       </c>
       <c r="B63">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="H63" s="9">
         <v>62</v>
@@ -6047,7 +6047,7 @@
       </c>
       <c r="B64">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="H64" s="9">
         <v>63</v>
@@ -6300,7 +6300,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -6358,15 +6358,15 @@
       </c>
       <c r="E2" s="6" t="str">
         <f ca="1">RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))</f>
-        <v>53 1 1</v>
+        <v>58 33 19</v>
       </c>
       <c r="F2" s="4">
         <f ca="1">RANDBETWEEN(MIN(CompetitionHost!$F:$F),MAX(CompetitionHost!$F:$F))</f>
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G2" s="4" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>45 39 52 33 31 5 8 42 41 13 17 21 15</v>
+        <v>6 13 16 26 9 38 6 44 46 50 45 32 42</v>
       </c>
       <c r="H2" s="11">
         <v>1</v>
@@ -6384,7 +6384,7 @@
       </c>
       <c r="E3" s="6" t="str">
         <f ca="1">RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))</f>
-        <v>18 58 54</v>
+        <v>7 13 12</v>
       </c>
       <c r="F3" s="4">
         <f ca="1">RANDBETWEEN(MIN(CompetitionHost!$F:$F),MAX(CompetitionHost!$F:$F))</f>
@@ -6392,7 +6392,7 @@
       </c>
       <c r="G3" s="4" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>10 9 31 22 8 20 26 49 30 39 46 7 39 29 35 8 30</v>
+        <v>21 23 13 25 44 43 5 43 46 16 5 46 27 23 47 15 39</v>
       </c>
       <c r="H3" s="11">
         <v>2</v>
@@ -6407,7 +6407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -6447,11 +6447,11 @@
       </c>
       <c r="C2" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>32 40 12 30 37</v>
+        <v>35 47 36 18 43</v>
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))</f>
-        <v>23 16 10</v>
+        <v>10 12 2</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>343</v>
@@ -6466,11 +6466,11 @@
       </c>
       <c r="C3" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>33 37 37 27 51</v>
+        <v>33 21 21 16 26</v>
       </c>
       <c r="D3" s="6" t="str">
         <f ca="1">RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))</f>
-        <v>55 5 40</v>
+        <v>52 28 14</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>346</v>
@@ -6485,11 +6485,11 @@
       </c>
       <c r="C4" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>10 51 24 23 17</v>
+        <v>46 39 9 41 5</v>
       </c>
       <c r="D4" s="6" t="str">
         <f ca="1">RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))</f>
-        <v>19 24 18</v>
+        <v>51 22 55</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>344</v>
@@ -6504,11 +6504,11 @@
       </c>
       <c r="C5" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>52 20 19 38 13</v>
+        <v>32 6 46 46 33</v>
       </c>
       <c r="D5" s="6" t="str">
         <f ca="1">RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))</f>
-        <v>1 15 7</v>
+        <v>27 26 60</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>345</v>

</xml_diff>

<commit_message>
I added some tabs on the Excel file
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="1875" tabRatio="709" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="1875" tabRatio="709" firstSheet="2" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="School" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,9 @@
     <sheet name="Notification" sheetId="11" r:id="rId8"/>
     <sheet name="User Page Buttons" sheetId="12" r:id="rId9"/>
     <sheet name="Home" sheetId="13" r:id="rId10"/>
-    <sheet name="Post" sheetId="10" r:id="rId11"/>
+    <sheet name="Company_from_User_POV" sheetId="14" r:id="rId11"/>
+    <sheet name="Competition_from_User_POV" sheetId="15" r:id="rId12"/>
+    <sheet name="Post" sheetId="10" r:id="rId13"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="392">
   <si>
     <t>Avila University</t>
   </si>
@@ -1149,9 +1151,6 @@
     <t>My Jobs</t>
   </si>
   <si>
-    <t>MSGS</t>
-  </si>
-  <si>
     <t>Notifications</t>
   </si>
   <si>
@@ -1171,6 +1170,48 @@
   </si>
   <si>
     <t>Profile Photo</t>
+  </si>
+  <si>
+    <t>About us</t>
+  </si>
+  <si>
+    <t>See job posts</t>
+  </si>
+  <si>
+    <t>Follow</t>
+  </si>
+  <si>
+    <t>Company picture</t>
+  </si>
+  <si>
+    <t>Tech Degrees needed</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>Company Name</t>
+  </si>
+  <si>
+    <t>Company Website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Every time you post something, I want you to have the option to post it on page only, or on tech feed </t>
+  </si>
+  <si>
+    <t>National Club Name</t>
+  </si>
+  <si>
+    <t>Events</t>
+  </si>
+  <si>
+    <t>National Club Website</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Picture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tech feed </t>
   </si>
 </sst>
 </file>
@@ -3185,10 +3226,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3198,14 +3239,15 @@
     <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>366</v>
       </c>
@@ -3222,39 +3264,42 @@
         <v>370</v>
       </c>
       <c r="F1" t="s">
+        <v>356</v>
+      </c>
+      <c r="G1" t="s">
         <v>371</v>
-      </c>
-      <c r="G1" t="s">
-        <v>372</v>
       </c>
       <c r="H1" t="s">
         <v>253</v>
       </c>
       <c r="I1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="J1" t="s">
+        <v>372</v>
+      </c>
+      <c r="K1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J2" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J3" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J4" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
         <v>376</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J5" t="s">
-        <v>377</v>
       </c>
     </row>
   </sheetData>
@@ -3264,10 +3309,169 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>384</v>
+      </c>
+      <c r="B1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C1" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>352</v>
+      </c>
+      <c r="B11" t="s">
+        <v>353</v>
+      </c>
+      <c r="C11" t="s">
+        <v>354</v>
+      </c>
+      <c r="D11" t="s">
+        <v>355</v>
+      </c>
+      <c r="E11" t="s">
+        <v>356</v>
+      </c>
+      <c r="F11" t="s">
+        <v>357</v>
+      </c>
+      <c r="G11" t="s">
+        <v>358</v>
+      </c>
+      <c r="H11" t="s">
+        <v>359</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>387</v>
+      </c>
+      <c r="B1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>352</v>
+      </c>
+      <c r="B10" t="s">
+        <v>353</v>
+      </c>
+      <c r="C10" t="s">
+        <v>354</v>
+      </c>
+      <c r="D10" t="s">
+        <v>355</v>
+      </c>
+      <c r="E10" t="s">
+        <v>356</v>
+      </c>
+      <c r="F10" t="s">
+        <v>357</v>
+      </c>
+      <c r="G10" t="s">
+        <v>358</v>
+      </c>
+      <c r="H10" t="s">
+        <v>359</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3527,7 +3731,7 @@
       </c>
       <c r="G2">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>3</v>
+        <v>106</v>
       </c>
       <c r="H2" s="9">
         <v>3</v>
@@ -3556,7 +3760,7 @@
       </c>
       <c r="G3">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>89</v>
+        <v>9</v>
       </c>
       <c r="H3" s="9">
         <v>4</v>
@@ -3585,7 +3789,7 @@
       </c>
       <c r="G4">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H4" s="9">
         <v>5</v>
@@ -3614,7 +3818,7 @@
       </c>
       <c r="G5">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>78</v>
+        <v>12</v>
       </c>
       <c r="H5" s="9">
         <v>6</v>
@@ -3643,7 +3847,7 @@
       </c>
       <c r="G6">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="H6" s="9">
         <v>7</v>
@@ -3672,7 +3876,7 @@
       </c>
       <c r="G7">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="H7" s="9">
         <v>8</v>
@@ -3701,7 +3905,7 @@
       </c>
       <c r="G8">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="H8" s="9">
         <v>9</v>
@@ -3730,7 +3934,7 @@
       </c>
       <c r="G9">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="H9" s="9">
         <v>10</v>
@@ -3759,7 +3963,7 @@
       </c>
       <c r="G10">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>101</v>
+        <v>27</v>
       </c>
       <c r="H10" s="9">
         <v>11</v>
@@ -3788,7 +3992,7 @@
       </c>
       <c r="G11">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="H11" s="9">
         <v>12</v>
@@ -3817,7 +4021,7 @@
       </c>
       <c r="G12">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>69</v>
+        <v>104</v>
       </c>
       <c r="H12" s="9">
         <v>13</v>
@@ -3846,7 +4050,7 @@
       </c>
       <c r="G13">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="H13" s="9">
         <v>14</v>
@@ -3875,7 +4079,7 @@
       </c>
       <c r="G14">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="H14" s="9">
         <v>15</v>
@@ -3904,7 +4108,7 @@
       </c>
       <c r="G15">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="H15" s="9">
         <v>16</v>
@@ -3933,7 +4137,7 @@
       </c>
       <c r="G16">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>71</v>
+        <v>2</v>
       </c>
       <c r="H16" s="9">
         <v>17</v>
@@ -3962,7 +4166,7 @@
       </c>
       <c r="G17">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="H17" s="9">
         <v>18</v>
@@ -3991,7 +4195,7 @@
       </c>
       <c r="G18">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>63</v>
+        <v>3</v>
       </c>
       <c r="H18" s="9">
         <v>19</v>
@@ -4020,7 +4224,7 @@
       </c>
       <c r="G19">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="H19" s="9">
         <v>20</v>
@@ -4049,7 +4253,7 @@
       </c>
       <c r="G20">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>106</v>
+        <v>40</v>
       </c>
       <c r="H20" s="9">
         <v>21</v>
@@ -4107,7 +4311,7 @@
       </c>
       <c r="G22">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="H22" s="9">
         <v>23</v>
@@ -4136,7 +4340,7 @@
       </c>
       <c r="G23">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>98</v>
+        <v>5</v>
       </c>
       <c r="H23" s="9">
         <v>24</v>
@@ -4165,7 +4369,7 @@
       </c>
       <c r="G24">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="H24" s="9">
         <v>25</v>
@@ -4194,7 +4398,7 @@
       </c>
       <c r="G25">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="H25" s="9">
         <v>26</v>
@@ -4223,7 +4427,7 @@
       </c>
       <c r="G26">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>69</v>
+        <v>108</v>
       </c>
       <c r="H26" s="9">
         <v>27</v>
@@ -4252,7 +4456,7 @@
       </c>
       <c r="G27">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>103</v>
+        <v>65</v>
       </c>
       <c r="H27" s="9">
         <v>28</v>
@@ -4281,7 +4485,7 @@
       </c>
       <c r="G28">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="H28" s="9">
         <v>29</v>
@@ -4310,7 +4514,7 @@
       </c>
       <c r="G29">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>10</v>
+        <v>111</v>
       </c>
       <c r="H29" s="9">
         <v>30</v>
@@ -4339,7 +4543,7 @@
       </c>
       <c r="G30">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H30" s="9">
         <v>31</v>
@@ -4368,7 +4572,7 @@
       </c>
       <c r="G31">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="H31" s="9">
         <v>32</v>
@@ -4397,7 +4601,7 @@
       </c>
       <c r="G32">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>85</v>
+        <v>46</v>
       </c>
       <c r="H32" s="9">
         <v>33</v>
@@ -4426,7 +4630,7 @@
       </c>
       <c r="G33">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>100</v>
+        <v>19</v>
       </c>
       <c r="H33" s="9">
         <v>34</v>
@@ -4455,7 +4659,7 @@
       </c>
       <c r="G34">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="H34" s="9">
         <v>35</v>
@@ -4484,7 +4688,7 @@
       </c>
       <c r="G35">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>110</v>
+        <v>57</v>
       </c>
       <c r="H35" s="9">
         <v>36</v>
@@ -4513,7 +4717,7 @@
       </c>
       <c r="G36">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="H36" s="9">
         <v>37</v>
@@ -4542,7 +4746,7 @@
       </c>
       <c r="G37">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="H37" s="9">
         <v>38</v>
@@ -4571,7 +4775,7 @@
       </c>
       <c r="G38">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="H38" s="9">
         <v>39</v>
@@ -4600,7 +4804,7 @@
       </c>
       <c r="G39">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>109</v>
+        <v>34</v>
       </c>
       <c r="H39" s="9">
         <v>40</v>
@@ -4629,7 +4833,7 @@
       </c>
       <c r="G40">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>87</v>
+        <v>18</v>
       </c>
       <c r="H40" s="9">
         <v>41</v>
@@ -4658,7 +4862,7 @@
       </c>
       <c r="G41">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H41" s="9">
         <v>42</v>
@@ -4687,7 +4891,7 @@
       </c>
       <c r="G42">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H42" s="9">
         <v>43</v>
@@ -4716,7 +4920,7 @@
       </c>
       <c r="G43">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>69</v>
+        <v>110</v>
       </c>
       <c r="H43" s="9">
         <v>44</v>
@@ -4745,7 +4949,7 @@
       </c>
       <c r="G44">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H44" s="9">
         <v>45</v>
@@ -4774,7 +4978,7 @@
       </c>
       <c r="G45">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="H45" s="9">
         <v>46</v>
@@ -4803,7 +5007,7 @@
       </c>
       <c r="G46">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="H46" s="9">
         <v>47</v>
@@ -4832,7 +5036,7 @@
       </c>
       <c r="G47">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="H47" s="9">
         <v>48</v>
@@ -4861,7 +5065,7 @@
       </c>
       <c r="G48">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="H48" s="9">
         <v>49</v>
@@ -4890,7 +5094,7 @@
       </c>
       <c r="G49">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H49" s="9">
         <v>50</v>
@@ -4919,7 +5123,7 @@
       </c>
       <c r="G50">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>9</v>
+        <v>107</v>
       </c>
       <c r="H50" s="9">
         <v>51</v>
@@ -4948,7 +5152,7 @@
       </c>
       <c r="G51">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="H51" s="9">
         <v>52</v>
@@ -5009,27 +5213,27 @@
       </c>
       <c r="B2">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="C2">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F2">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G2" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>44 19 49 51 9</v>
+        <v>48 10 52 38 42</v>
       </c>
       <c r="H2" s="9">
         <v>1</v>
@@ -5041,27 +5245,27 @@
       </c>
       <c r="B3">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="C3">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="E3">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F3">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="G3" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>36 38 8 8 28</v>
+        <v>11 16 48 5 49</v>
       </c>
       <c r="H3" s="9">
         <v>2</v>
@@ -5073,27 +5277,27 @@
       </c>
       <c r="B4">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="D4">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E4">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="F4">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="G4" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>12 22 8 27 26</v>
+        <v>41 37 38 7 48</v>
       </c>
       <c r="H4" s="9">
         <v>3</v>
@@ -5105,27 +5309,27 @@
       </c>
       <c r="B5">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D5">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="E5">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="F5">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="G5" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>48 45 5 6 30</v>
+        <v>3 21 39 14 12</v>
       </c>
       <c r="H5" s="9">
         <v>4</v>
@@ -5137,27 +5341,27 @@
       </c>
       <c r="B6">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="C6">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E6">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F6">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="G6" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>27 7 23 13 14</v>
+        <v>17 17 37 17 43</v>
       </c>
       <c r="H6" s="9">
         <v>5</v>
@@ -5169,27 +5373,27 @@
       </c>
       <c r="B7">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
+        <v>82</v>
+      </c>
+      <c r="C7">
+        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
         <v>37</v>
       </c>
-      <c r="C7">
-        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>9</v>
-      </c>
       <c r="D7">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="E7">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G7" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>16 19 44 20 26</v>
+        <v>32 37 44 27 18</v>
       </c>
       <c r="H7" s="9">
         <v>6</v>
@@ -5201,27 +5405,27 @@
       </c>
       <c r="B8">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="C8">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="D8">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="E8">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="F8">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="G8" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>29 28 8 37 20</v>
+        <v>23 6 21 23 13</v>
       </c>
       <c r="H8" s="9">
         <v>7</v>
@@ -5233,27 +5437,27 @@
       </c>
       <c r="B9">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="C9">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D9">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="E9">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="F9">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G9" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>32 8 36 40 25</v>
+        <v>38 20 8 31 32</v>
       </c>
       <c r="H9" s="9">
         <v>8</v>
@@ -5265,27 +5469,27 @@
       </c>
       <c r="B10">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C10">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="D10">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="E10">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
+        <v>45</v>
+      </c>
+      <c r="F10">
+        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
         <v>23</v>
-      </c>
-      <c r="F10">
-        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>27</v>
       </c>
       <c r="G10" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>9 51 49 41 43</v>
+        <v>33 14 16 8 51</v>
       </c>
       <c r="H10" s="9">
         <v>9</v>
@@ -5297,27 +5501,27 @@
       </c>
       <c r="B11">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C11">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="D11">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E11">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="F11">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G11" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>39 40 10 47 24</v>
+        <v>22 9 11 20 46</v>
       </c>
       <c r="H11" s="9">
         <v>10</v>
@@ -5329,27 +5533,27 @@
       </c>
       <c r="B12">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="C12">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="D12">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E12">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="F12">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G12" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>31 43 50 33 43</v>
+        <v>31 10 21 45 28</v>
       </c>
       <c r="H12" s="9">
         <v>11</v>
@@ -5361,27 +5565,27 @@
       </c>
       <c r="B13">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
+        <v>41</v>
+      </c>
+      <c r="C13">
+        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
         <v>18</v>
       </c>
-      <c r="C13">
-        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>13</v>
-      </c>
       <c r="D13">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="E13">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F13">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G13" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>14 9 36 11 51</v>
+        <v>31 27 13 40 11</v>
       </c>
       <c r="H13" s="9">
         <v>12</v>
@@ -5393,11 +5597,11 @@
       </c>
       <c r="B14">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="C14">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D14">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
@@ -5405,15 +5609,15 @@
       </c>
       <c r="E14">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F14">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="G14" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>15 35 21 48 40</v>
+        <v>43 10 25 18 49</v>
       </c>
       <c r="H14" s="9">
         <v>13</v>
@@ -5425,27 +5629,27 @@
       </c>
       <c r="B15">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="C15">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D15">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E15">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="F15">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="G15" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>47 6 12 31 24</v>
+        <v>38 19 45 19 30</v>
       </c>
       <c r="H15" s="9">
         <v>14</v>
@@ -5457,27 +5661,27 @@
       </c>
       <c r="B16">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>102</v>
+        <v>34</v>
       </c>
       <c r="C16">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D16">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="E16">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="F16">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="G16" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>29 5 4 8 16</v>
+        <v>28 24 35 49 18</v>
       </c>
       <c r="H16" s="9">
         <v>15</v>
@@ -5489,27 +5693,27 @@
       </c>
       <c r="B17">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>103</v>
+        <v>30</v>
       </c>
       <c r="C17">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D17">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E17">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="F17">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G17" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>8 17 24 40 10</v>
+        <v>34 33 49 13 45</v>
       </c>
       <c r="H17" s="9">
         <v>16</v>
@@ -5521,27 +5725,27 @@
       </c>
       <c r="B18">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>110</v>
+        <v>36</v>
       </c>
       <c r="C18">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D18">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
+        <v>41</v>
+      </c>
+      <c r="E18">
+        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
+        <v>19</v>
+      </c>
+      <c r="F18">
+        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
         <v>42</v>
-      </c>
-      <c r="E18">
-        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>39</v>
-      </c>
-      <c r="F18">
-        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>20</v>
       </c>
       <c r="G18" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>5 25 29 30 13</v>
+        <v>25 42 43 5 11</v>
       </c>
       <c r="H18" s="9">
         <v>17</v>
@@ -5553,27 +5757,27 @@
       </c>
       <c r="B19">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>6</v>
+        <v>83</v>
       </c>
       <c r="C19">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D19">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="E19">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F19">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="G19" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>26 7 29 36 27</v>
+        <v>29 9 5 28 38</v>
       </c>
       <c r="H19" s="9">
         <v>18</v>
@@ -5585,27 +5789,27 @@
       </c>
       <c r="B20">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
+        <v>65</v>
+      </c>
+      <c r="C20">
+        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
+        <v>13</v>
+      </c>
+      <c r="D20">
+        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
         <v>42</v>
       </c>
-      <c r="C20">
-        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>17</v>
-      </c>
-      <c r="D20">
+      <c r="E20">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
         <v>34</v>
       </c>
-      <c r="E20">
-        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>39</v>
-      </c>
       <c r="F20">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="G20" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>3 37 37 24 8</v>
+        <v>29 11 41 38 29</v>
       </c>
       <c r="H20" s="9">
         <v>19</v>
@@ -5617,27 +5821,27 @@
       </c>
       <c r="B21">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>101</v>
+        <v>18</v>
       </c>
       <c r="C21">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D21">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="E21">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="F21">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="G21" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>46 4 52 35 44</v>
+        <v>13 51 10 41 8</v>
       </c>
       <c r="H21" s="9">
         <v>20</v>
@@ -5649,27 +5853,27 @@
       </c>
       <c r="B22">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="C22">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D22">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="E22">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="F22">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="G22" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>50 50 6 42 13</v>
+        <v>46 17 23 50 28</v>
       </c>
       <c r="H22" s="9">
         <v>21</v>
@@ -5681,27 +5885,27 @@
       </c>
       <c r="B23">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>89</v>
+        <v>4</v>
       </c>
       <c r="C23">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="D23">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E23">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="F23">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="G23" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>15 52 3 25 6</v>
+        <v>32 32 4 8 7</v>
       </c>
       <c r="H23" s="9">
         <v>22</v>
@@ -5713,11 +5917,11 @@
       </c>
       <c r="B24">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>96</v>
+        <v>25</v>
       </c>
       <c r="G24" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>40 23 15 32 46</v>
+        <v>26 18 7 32 35</v>
       </c>
       <c r="H24" s="9">
         <v>23</v>
@@ -5729,11 +5933,11 @@
       </c>
       <c r="B25">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>37</v>
+        <v>101</v>
       </c>
       <c r="G25" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>25 24 45 35 35</v>
+        <v>26 22 32 27 12</v>
       </c>
       <c r="H25" s="9">
         <v>24</v>
@@ -5745,11 +5949,11 @@
       </c>
       <c r="B26">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="G26" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>49 52 9 24 44</v>
+        <v>27 12 34 25 17</v>
       </c>
       <c r="H26" s="9">
         <v>25</v>
@@ -5761,11 +5965,11 @@
       </c>
       <c r="B27">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="G27" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>48 47 11 19 28</v>
+        <v>33 28 33 38 40</v>
       </c>
       <c r="H27" s="9">
         <v>26</v>
@@ -5777,11 +5981,11 @@
       </c>
       <c r="B28">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>23</v>
+        <v>89</v>
       </c>
       <c r="G28" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>52 18 45 16 27</v>
+        <v>31 41 50 24 21</v>
       </c>
       <c r="H28" s="9">
         <v>27</v>
@@ -5793,11 +5997,11 @@
       </c>
       <c r="B29">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="G29" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>38 33 45 36 9</v>
+        <v>36 44 26 12 47</v>
       </c>
       <c r="H29" s="9">
         <v>28</v>
@@ -5809,11 +6013,11 @@
       </c>
       <c r="B30">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>58</v>
+        <v>96</v>
       </c>
       <c r="G30" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>44 26 15 11 49</v>
+        <v>13 9 37 4 27</v>
       </c>
       <c r="H30" s="9">
         <v>29</v>
@@ -5825,11 +6029,11 @@
       </c>
       <c r="B31">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>33</v>
+        <v>110</v>
       </c>
       <c r="G31" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>16 6 10 18 16</v>
+        <v>46 38 17 39 41</v>
       </c>
       <c r="H31" s="9">
         <v>30</v>
@@ -5841,11 +6045,11 @@
       </c>
       <c r="B32">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="G32" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>26 16 41 26 31</v>
+        <v>13 25 30 16 40</v>
       </c>
       <c r="H32" s="9">
         <v>31</v>
@@ -5857,11 +6061,11 @@
       </c>
       <c r="B33">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>91</v>
+        <v>20</v>
       </c>
       <c r="G33" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>48 48 39 47 4</v>
+        <v>12 25 37 13 34</v>
       </c>
       <c r="H33" s="9">
         <v>32</v>
@@ -5873,11 +6077,11 @@
       </c>
       <c r="B34">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="G34" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>29 21 43 7 34</v>
+        <v>51 50 21 13 28</v>
       </c>
       <c r="H34" s="9">
         <v>33</v>
@@ -5889,11 +6093,11 @@
       </c>
       <c r="B35">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G35" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>52 44 4 20 25</v>
+        <v>18 22 13 10 41</v>
       </c>
       <c r="H35" s="9">
         <v>34</v>
@@ -5905,11 +6109,11 @@
       </c>
       <c r="B36">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="G36" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>29 13 20 38 24</v>
+        <v>7 18 48 45 16</v>
       </c>
       <c r="H36" s="9">
         <v>35</v>
@@ -5921,11 +6125,11 @@
       </c>
       <c r="B37">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="G37" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>49 14 10 11 27</v>
+        <v>39 11 41 5 50</v>
       </c>
       <c r="H37" s="9">
         <v>36</v>
@@ -5937,11 +6141,11 @@
       </c>
       <c r="B38">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>111</v>
+        <v>33</v>
       </c>
       <c r="G38" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>38 33 5 40 49</v>
+        <v>24 44 33 47 9</v>
       </c>
       <c r="H38" s="9">
         <v>37</v>
@@ -5953,11 +6157,11 @@
       </c>
       <c r="B39">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>62</v>
+        <v>7</v>
       </c>
       <c r="G39" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>43 14 47 5 44</v>
+        <v>29 46 31 47 31</v>
       </c>
       <c r="H39" s="9">
         <v>38</v>
@@ -5969,11 +6173,11 @@
       </c>
       <c r="B40">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>112</v>
+        <v>32</v>
       </c>
       <c r="G40" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>3 46 34 13 21</v>
+        <v>8 8 8 4 40</v>
       </c>
       <c r="H40" s="9">
         <v>39</v>
@@ -5985,11 +6189,11 @@
       </c>
       <c r="B41">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="G41" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>31 17 34 21 46</v>
+        <v>34 26 36 5 11</v>
       </c>
       <c r="H41" s="9">
         <v>40</v>
@@ -6001,11 +6205,11 @@
       </c>
       <c r="B42">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>52</v>
+        <v>105</v>
       </c>
       <c r="G42" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>21 8 45 5 17</v>
+        <v>42 7 29 50 27</v>
       </c>
       <c r="H42" s="9">
         <v>41</v>
@@ -6017,11 +6221,11 @@
       </c>
       <c r="B43">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="G43" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>47 8 8 50 38</v>
+        <v>26 37 27 18 18</v>
       </c>
       <c r="H43" s="9">
         <v>42</v>
@@ -6033,11 +6237,11 @@
       </c>
       <c r="B44">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>109</v>
+        <v>69</v>
       </c>
       <c r="G44" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>13 3 6 37 50</v>
+        <v>9 9 7 44 45</v>
       </c>
       <c r="H44" s="9">
         <v>43</v>
@@ -6049,11 +6253,11 @@
       </c>
       <c r="B45">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="G45" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>10 30 15 44 39</v>
+        <v>31 13 7 44 5</v>
       </c>
       <c r="H45" s="9">
         <v>44</v>
@@ -6065,11 +6269,11 @@
       </c>
       <c r="B46">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="G46" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>24 26 43 36 49</v>
+        <v>22 12 18 48 12</v>
       </c>
       <c r="H46" s="9">
         <v>45</v>
@@ -6081,11 +6285,11 @@
       </c>
       <c r="B47">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="G47" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>5 11 12 49 30</v>
+        <v>12 24 45 46 8</v>
       </c>
       <c r="H47" s="9">
         <v>46</v>
@@ -6097,11 +6301,11 @@
       </c>
       <c r="B48">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>79</v>
+        <v>28</v>
       </c>
       <c r="G48" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>18 26 24 18 44</v>
+        <v>10 11 13 7 41</v>
       </c>
       <c r="H48" s="9">
         <v>47</v>
@@ -6113,11 +6317,11 @@
       </c>
       <c r="B49">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>104</v>
+        <v>47</v>
       </c>
       <c r="G49" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>12 14 35 38 21</v>
+        <v>14 49 32 20 39</v>
       </c>
       <c r="H49" s="9">
         <v>48</v>
@@ -6129,11 +6333,11 @@
       </c>
       <c r="B50">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="G50" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>28 26 38 50 16</v>
+        <v>49 10 37 42 20</v>
       </c>
       <c r="H50" s="9">
         <v>49</v>
@@ -6145,11 +6349,11 @@
       </c>
       <c r="B51">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G51" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>52 30 50 51 14</v>
+        <v>7 22 9 51 24</v>
       </c>
       <c r="H51" s="9">
         <v>50</v>
@@ -6161,11 +6365,11 @@
       </c>
       <c r="B52">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="G52" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>16 46 14 46 45</v>
+        <v>3 45 32 41 26</v>
       </c>
       <c r="H52" s="9">
         <v>51</v>
@@ -6177,11 +6381,11 @@
       </c>
       <c r="B53">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="G53" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>48 4 34 7 8</v>
+        <v>42 19 31 43 18</v>
       </c>
       <c r="H53" s="9">
         <v>52</v>
@@ -6193,11 +6397,11 @@
       </c>
       <c r="B54">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G54" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>52 25 37 40 38</v>
+        <v>43 28 13 40 5</v>
       </c>
       <c r="H54" s="9">
         <v>53</v>
@@ -6209,11 +6413,11 @@
       </c>
       <c r="B55">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="G55" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>30 38 40 17 24</v>
+        <v>11 8 31 6 23</v>
       </c>
       <c r="H55" s="9">
         <v>54</v>
@@ -6225,11 +6429,11 @@
       </c>
       <c r="B56">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>107</v>
+        <v>11</v>
       </c>
       <c r="G56" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>12 10 39 47 3</v>
+        <v>30 22 39 21 26</v>
       </c>
       <c r="H56" s="9">
         <v>55</v>
@@ -6241,11 +6445,11 @@
       </c>
       <c r="B57">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="G57" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>22 46 30 45 31</v>
+        <v>21 45 31 44 42</v>
       </c>
       <c r="H57" s="9">
         <v>56</v>
@@ -6257,11 +6461,11 @@
       </c>
       <c r="B58">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="G58" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>9 5 7 24 35</v>
+        <v>22 43 47 14 44</v>
       </c>
       <c r="H58" s="9">
         <v>57</v>
@@ -6273,7 +6477,7 @@
       </c>
       <c r="B59">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="H59" s="9">
         <v>58</v>
@@ -6285,7 +6489,7 @@
       </c>
       <c r="B60">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="H60" s="9">
         <v>59</v>
@@ -6297,7 +6501,7 @@
       </c>
       <c r="B61">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="H61" s="9">
         <v>60</v>
@@ -6309,7 +6513,7 @@
       </c>
       <c r="B62">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H62" s="9">
         <v>61</v>
@@ -6321,7 +6525,7 @@
       </c>
       <c r="B63">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>100</v>
+        <v>66</v>
       </c>
       <c r="H63" s="9">
         <v>62</v>
@@ -6333,7 +6537,7 @@
       </c>
       <c r="B64">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="H64" s="9">
         <v>63</v>
@@ -6644,7 +6848,7 @@
       </c>
       <c r="E2" s="6" t="str">
         <f ca="1">RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))</f>
-        <v>10 11 51</v>
+        <v>51 14 2</v>
       </c>
       <c r="F2" s="4">
         <f ca="1">RANDBETWEEN(MIN(CompetitionHost!$F:$F),MAX(CompetitionHost!$F:$F))</f>
@@ -6652,7 +6856,7 @@
       </c>
       <c r="G2" s="4" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>10 20 39 22 11 13 33 4 15 46 5 12 44</v>
+        <v>23 5 34 45 35 32 22 9 49 19 9 43 3</v>
       </c>
       <c r="H2" s="11">
         <v>1</v>
@@ -6670,15 +6874,15 @@
       </c>
       <c r="E3" s="6" t="str">
         <f ca="1">RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))</f>
-        <v>15 2 14</v>
+        <v>56 39 30</v>
       </c>
       <c r="F3" s="4">
         <f ca="1">RANDBETWEEN(MIN(CompetitionHost!$F:$F),MAX(CompetitionHost!$F:$F))</f>
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G3" s="4" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>52 36 19 10 36 43 47 34 43 35 32 10 20 6 32 25 12</v>
+        <v>41 40 23 35 18 33 41 21 36 22 23 37 10 32 31 44 52</v>
       </c>
       <c r="H3" s="11">
         <v>2</v>
@@ -6756,11 +6960,11 @@
       </c>
       <c r="C2" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>21 29 31 3 8</v>
+        <v>40 7 19 7 12</v>
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))</f>
-        <v>21 10 60</v>
+        <v>27 13 1</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>343</v>
@@ -6775,11 +6979,11 @@
       </c>
       <c r="C3" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>13 40 14 50 43</v>
+        <v>8 38 23 30 47</v>
       </c>
       <c r="D3" s="6" t="str">
         <f ca="1">RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))</f>
-        <v>59 39 36</v>
+        <v>54 43 26</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>346</v>
@@ -6794,11 +6998,11 @@
       </c>
       <c r="C4" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>4 6 26 20 28</v>
+        <v>43 11 28 3 30</v>
       </c>
       <c r="D4" s="6" t="str">
         <f ca="1">RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))</f>
-        <v>22 35 13</v>
+        <v>25 57 18</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>344</v>
@@ -6813,11 +7017,11 @@
       </c>
       <c r="C5" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>24 29 47 18 4</v>
+        <v>52 37 48 8 25</v>
       </c>
       <c r="D5" s="6" t="str">
         <f ca="1">RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))</f>
-        <v>31 16 20</v>
+        <v>18 35 7</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>345</v>
@@ -6834,10 +7038,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6849,7 +7053,7 @@
     <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
@@ -6901,6 +7105,11 @@
         <v>363</v>
       </c>
     </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>386</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Hopefully this does not mess up our file.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="1875" tabRatio="709" firstSheet="2" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="1875" tabRatio="855" firstSheet="2" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="School" sheetId="2" r:id="rId1"/>
@@ -23,8 +23,10 @@
     <sheet name="User Page Buttons" sheetId="12" r:id="rId9"/>
     <sheet name="Home" sheetId="13" r:id="rId10"/>
     <sheet name="Company_from_User_POV" sheetId="14" r:id="rId11"/>
-    <sheet name="Competition_from_User_POV" sheetId="15" r:id="rId12"/>
-    <sheet name="Post" sheetId="10" r:id="rId13"/>
+    <sheet name="Messages" sheetId="16" r:id="rId12"/>
+    <sheet name="Sheet2" sheetId="17" r:id="rId13"/>
+    <sheet name="Competition_from_User_POV" sheetId="15" r:id="rId14"/>
+    <sheet name="Post" sheetId="10" r:id="rId15"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="429">
   <si>
     <t>Avila University</t>
   </si>
@@ -1212,6 +1214,117 @@
   </si>
   <si>
     <t xml:space="preserve">Tech feed </t>
+  </si>
+  <si>
+    <t>Aerospace, Aeronautical and Astronautical Engineering</t>
+  </si>
+  <si>
+    <t>Agricultural Engineering</t>
+  </si>
+  <si>
+    <t>Architectural Engineering</t>
+  </si>
+  <si>
+    <t>Biochemical Engineering</t>
+  </si>
+  <si>
+    <t>Biological/Biosystems Engineering</t>
+  </si>
+  <si>
+    <t>Biomedical/Medical Engineering</t>
+  </si>
+  <si>
+    <t>Ceramic Sciences and Engineering</t>
+  </si>
+  <si>
+    <t>Chemical Engineering</t>
+  </si>
+  <si>
+    <t>Civil Engineering</t>
+  </si>
+  <si>
+    <t>Computer Engineering</t>
+  </si>
+  <si>
+    <t>Construction Engineering</t>
+  </si>
+  <si>
+    <t>Electrical, Electronics and Communications Engineering</t>
+  </si>
+  <si>
+    <t>Electromechanical Engineering</t>
+  </si>
+  <si>
+    <t>Engineering Chemistry</t>
+  </si>
+  <si>
+    <t>Engineering Mechanics</t>
+  </si>
+  <si>
+    <t>Engineering Physics</t>
+  </si>
+  <si>
+    <t>Engineering Science</t>
+  </si>
+  <si>
+    <t>Environmental/Environmental Health Engineering</t>
+  </si>
+  <si>
+    <t>Forest Engineering</t>
+  </si>
+  <si>
+    <t>Geological/Geophysical Engineering</t>
+  </si>
+  <si>
+    <t>Industrial Engineering</t>
+  </si>
+  <si>
+    <t>Manufacturing Engineering</t>
+  </si>
+  <si>
+    <t>Materials Engineering</t>
+  </si>
+  <si>
+    <t>Mechanical Engineering</t>
+  </si>
+  <si>
+    <t>Mechatronics, Robotics, and Automation Engineering</t>
+  </si>
+  <si>
+    <t>Metallurgical Engineering</t>
+  </si>
+  <si>
+    <t>Mining and Mineral Engineering</t>
+  </si>
+  <si>
+    <t>Naval Architecture and Marine Engineering</t>
+  </si>
+  <si>
+    <t>Nuclear Engineering</t>
+  </si>
+  <si>
+    <t>Ocean Engineering</t>
+  </si>
+  <si>
+    <t>Operations Research</t>
+  </si>
+  <si>
+    <t>Paper Science and Engineering</t>
+  </si>
+  <si>
+    <t>Petroleum Engineering</t>
+  </si>
+  <si>
+    <t>Polymer/Plastics Engineering</t>
+  </si>
+  <si>
+    <t>Surveying Engineering</t>
+  </si>
+  <si>
+    <t>Systems Engineering</t>
+  </si>
+  <si>
+    <t>Textile Scienc</t>
   </si>
 </sst>
 </file>
@@ -3394,9 +3507,228 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R25" sqref="R25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>428</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -3466,7 +3798,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -3731,7 +4063,7 @@
       </c>
       <c r="G2">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="H2" s="9">
         <v>3</v>
@@ -3760,7 +4092,7 @@
       </c>
       <c r="G3">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="H3" s="9">
         <v>4</v>
@@ -3789,7 +4121,7 @@
       </c>
       <c r="G4">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>111</v>
+        <v>46</v>
       </c>
       <c r="H4" s="9">
         <v>5</v>
@@ -3818,7 +4150,7 @@
       </c>
       <c r="G5">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="H5" s="9">
         <v>6</v>
@@ -3847,7 +4179,7 @@
       </c>
       <c r="G6">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="H6" s="9">
         <v>7</v>
@@ -3876,7 +4208,7 @@
       </c>
       <c r="G7">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="H7" s="9">
         <v>8</v>
@@ -3905,7 +4237,7 @@
       </c>
       <c r="G8">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="H8" s="9">
         <v>9</v>
@@ -3934,7 +4266,7 @@
       </c>
       <c r="G9">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="H9" s="9">
         <v>10</v>
@@ -3963,7 +4295,7 @@
       </c>
       <c r="G10">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="H10" s="9">
         <v>11</v>
@@ -3992,7 +4324,7 @@
       </c>
       <c r="G11">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>105</v>
+        <v>24</v>
       </c>
       <c r="H11" s="9">
         <v>12</v>
@@ -4021,7 +4353,7 @@
       </c>
       <c r="G12">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>104</v>
+        <v>44</v>
       </c>
       <c r="H12" s="9">
         <v>13</v>
@@ -4050,7 +4382,7 @@
       </c>
       <c r="G13">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="H13" s="9">
         <v>14</v>
@@ -4079,7 +4411,7 @@
       </c>
       <c r="G14">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="H14" s="9">
         <v>15</v>
@@ -4108,7 +4440,7 @@
       </c>
       <c r="G15">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="H15" s="9">
         <v>16</v>
@@ -4137,7 +4469,7 @@
       </c>
       <c r="G16">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>2</v>
+        <v>107</v>
       </c>
       <c r="H16" s="9">
         <v>17</v>
@@ -4166,7 +4498,7 @@
       </c>
       <c r="G17">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="H17" s="9">
         <v>18</v>
@@ -4195,7 +4527,7 @@
       </c>
       <c r="G18">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="H18" s="9">
         <v>19</v>
@@ -4224,7 +4556,7 @@
       </c>
       <c r="G19">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="H19" s="9">
         <v>20</v>
@@ -4253,7 +4585,7 @@
       </c>
       <c r="G20">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="H20" s="9">
         <v>21</v>
@@ -4282,7 +4614,7 @@
       </c>
       <c r="G21">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="H21" s="9">
         <v>22</v>
@@ -4311,7 +4643,7 @@
       </c>
       <c r="G22">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>90</v>
+        <v>38</v>
       </c>
       <c r="H22" s="9">
         <v>23</v>
@@ -4340,7 +4672,7 @@
       </c>
       <c r="G23">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>5</v>
+        <v>89</v>
       </c>
       <c r="H23" s="9">
         <v>24</v>
@@ -4369,7 +4701,7 @@
       </c>
       <c r="G24">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>52</v>
+        <v>97</v>
       </c>
       <c r="H24" s="9">
         <v>25</v>
@@ -4398,7 +4730,7 @@
       </c>
       <c r="G25">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="H25" s="9">
         <v>26</v>
@@ -4427,7 +4759,7 @@
       </c>
       <c r="G26">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>108</v>
+        <v>70</v>
       </c>
       <c r="H26" s="9">
         <v>27</v>
@@ -4456,7 +4788,7 @@
       </c>
       <c r="G27">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>65</v>
+        <v>113</v>
       </c>
       <c r="H27" s="9">
         <v>28</v>
@@ -4485,7 +4817,7 @@
       </c>
       <c r="G28">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H28" s="9">
         <v>29</v>
@@ -4514,7 +4846,7 @@
       </c>
       <c r="G29">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>111</v>
+        <v>28</v>
       </c>
       <c r="H29" s="9">
         <v>30</v>
@@ -4543,7 +4875,7 @@
       </c>
       <c r="G30">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="H30" s="9">
         <v>31</v>
@@ -4572,7 +4904,7 @@
       </c>
       <c r="G31">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="H31" s="9">
         <v>32</v>
@@ -4601,7 +4933,7 @@
       </c>
       <c r="G32">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>46</v>
+        <v>109</v>
       </c>
       <c r="H32" s="9">
         <v>33</v>
@@ -4630,7 +4962,7 @@
       </c>
       <c r="G33">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="H33" s="9">
         <v>34</v>
@@ -4659,7 +4991,7 @@
       </c>
       <c r="G34">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="H34" s="9">
         <v>35</v>
@@ -4688,7 +5020,7 @@
       </c>
       <c r="G35">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>57</v>
+        <v>85</v>
       </c>
       <c r="H35" s="9">
         <v>36</v>
@@ -4717,7 +5049,7 @@
       </c>
       <c r="G36">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="H36" s="9">
         <v>37</v>
@@ -4746,7 +5078,7 @@
       </c>
       <c r="G37">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="H37" s="9">
         <v>38</v>
@@ -4775,7 +5107,7 @@
       </c>
       <c r="G38">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="H38" s="9">
         <v>39</v>
@@ -4804,7 +5136,7 @@
       </c>
       <c r="G39">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="H39" s="9">
         <v>40</v>
@@ -4833,7 +5165,7 @@
       </c>
       <c r="G40">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>18</v>
+        <v>99</v>
       </c>
       <c r="H40" s="9">
         <v>41</v>
@@ -4862,7 +5194,7 @@
       </c>
       <c r="G41">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="H41" s="9">
         <v>42</v>
@@ -4891,7 +5223,7 @@
       </c>
       <c r="G42">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>90</v>
+        <v>19</v>
       </c>
       <c r="H42" s="9">
         <v>43</v>
@@ -4920,7 +5252,7 @@
       </c>
       <c r="G43">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="H43" s="9">
         <v>44</v>
@@ -4949,7 +5281,7 @@
       </c>
       <c r="G44">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H44" s="9">
         <v>45</v>
@@ -4978,7 +5310,7 @@
       </c>
       <c r="G45">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>74</v>
+        <v>18</v>
       </c>
       <c r="H45" s="9">
         <v>46</v>
@@ -5007,7 +5339,7 @@
       </c>
       <c r="G46">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>100</v>
+        <v>46</v>
       </c>
       <c r="H46" s="9">
         <v>47</v>
@@ -5036,7 +5368,7 @@
       </c>
       <c r="G47">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>55</v>
+        <v>101</v>
       </c>
       <c r="H47" s="9">
         <v>48</v>
@@ -5065,7 +5397,7 @@
       </c>
       <c r="G48">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="H48" s="9">
         <v>49</v>
@@ -5094,7 +5426,7 @@
       </c>
       <c r="G49">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="H49" s="9">
         <v>50</v>
@@ -5123,7 +5455,7 @@
       </c>
       <c r="G50">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>107</v>
+        <v>35</v>
       </c>
       <c r="H50" s="9">
         <v>51</v>
@@ -5152,7 +5484,7 @@
       </c>
       <c r="G51">
         <f ca="1">RANDBETWEEN(MIN(School!D:D),MAX(School!D:D))</f>
-        <v>90</v>
+        <v>25</v>
       </c>
       <c r="H51" s="9">
         <v>52</v>
@@ -5213,27 +5545,27 @@
       </c>
       <c r="B2">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
+        <v>94</v>
+      </c>
+      <c r="C2">
+        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
         <v>41</v>
       </c>
-      <c r="C2">
-        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>27</v>
-      </c>
-      <c r="D2">
-        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>47</v>
-      </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
         <v>33</v>
-      </c>
-      <c r="F2">
-        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>6</v>
       </c>
       <c r="G2" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>48 10 52 38 42</v>
+        <v>10 38 52 10 47</v>
       </c>
       <c r="H2" s="9">
         <v>1</v>
@@ -5245,27 +5577,27 @@
       </c>
       <c r="B3">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E3">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="F3">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G3" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>11 16 48 5 49</v>
+        <v>4 38 29 34 28</v>
       </c>
       <c r="H3" s="9">
         <v>2</v>
@@ -5277,27 +5609,27 @@
       </c>
       <c r="B4">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>28</v>
+        <v>89</v>
       </c>
       <c r="C4">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D4">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="E4">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F4">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="G4" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>41 37 38 7 48</v>
+        <v>15 45 48 12 19</v>
       </c>
       <c r="H4" s="9">
         <v>3</v>
@@ -5309,27 +5641,27 @@
       </c>
       <c r="B5">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>17</v>
+        <v>108</v>
       </c>
       <c r="C5">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D5">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E5">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="F5">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="G5" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>3 21 39 14 12</v>
+        <v>40 43 39 26 8</v>
       </c>
       <c r="H5" s="9">
         <v>4</v>
@@ -5341,27 +5673,27 @@
       </c>
       <c r="B6">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>111</v>
+        <v>44</v>
       </c>
       <c r="C6">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D6">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="E6">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="F6">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G6" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>17 17 37 17 43</v>
+        <v>42 20 37 11 28</v>
       </c>
       <c r="H6" s="9">
         <v>5</v>
@@ -5373,19 +5705,19 @@
       </c>
       <c r="B7">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="C7">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D7">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E7">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F7">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
@@ -5393,7 +5725,7 @@
       </c>
       <c r="G7" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>32 37 44 27 18</v>
+        <v>13 34 14 19 10</v>
       </c>
       <c r="H7" s="9">
         <v>6</v>
@@ -5405,27 +5737,27 @@
       </c>
       <c r="B8">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="C8">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D8">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E8">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="F8">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G8" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>23 6 21 23 13</v>
+        <v>10 10 48 10 49</v>
       </c>
       <c r="H8" s="9">
         <v>7</v>
@@ -5437,27 +5769,27 @@
       </c>
       <c r="B9">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C9">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="D9">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="E9">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F9">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G9" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>38 20 8 31 32</v>
+        <v>19 6 32 15 40</v>
       </c>
       <c r="H9" s="9">
         <v>8</v>
@@ -5469,27 +5801,27 @@
       </c>
       <c r="B10">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="C10">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D10">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E10">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="F10">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G10" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>33 14 16 8 51</v>
+        <v>15 46 46 39 13</v>
       </c>
       <c r="H10" s="9">
         <v>9</v>
@@ -5501,27 +5833,27 @@
       </c>
       <c r="B11">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C11">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D11">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="E11">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="F11">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="G11" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>22 9 11 20 46</v>
+        <v>33 13 50 36 7</v>
       </c>
       <c r="H11" s="9">
         <v>10</v>
@@ -5533,27 +5865,27 @@
       </c>
       <c r="B12">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C12">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="D12">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="E12">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F12">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="G12" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>31 10 21 45 28</v>
+        <v>14 43 28 18 52</v>
       </c>
       <c r="H12" s="9">
         <v>11</v>
@@ -5565,27 +5897,27 @@
       </c>
       <c r="B13">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>41</v>
+        <v>96</v>
       </c>
       <c r="C13">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D13">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="E13">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="F13">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="G13" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>31 27 13 40 11</v>
+        <v>22 6 15 6 37</v>
       </c>
       <c r="H13" s="9">
         <v>12</v>
@@ -5597,27 +5929,27 @@
       </c>
       <c r="B14">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>75</v>
+        <v>17</v>
       </c>
       <c r="C14">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="D14">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="E14">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="F14">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="G14" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>43 10 25 18 49</v>
+        <v>6 27 24 42 41</v>
       </c>
       <c r="H14" s="9">
         <v>13</v>
@@ -5629,27 +5961,27 @@
       </c>
       <c r="B15">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="C15">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="D15">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E15">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="F15">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="G15" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>38 19 45 19 30</v>
+        <v>4 16 46 29 13</v>
       </c>
       <c r="H15" s="9">
         <v>14</v>
@@ -5661,27 +5993,27 @@
       </c>
       <c r="B16">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="C16">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="D16">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="E16">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
+        <v>37</v>
+      </c>
+      <c r="F16">
+        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
         <v>23</v>
-      </c>
-      <c r="F16">
-        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>3</v>
       </c>
       <c r="G16" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>28 24 35 49 18</v>
+        <v>10 51 51 51 23</v>
       </c>
       <c r="H16" s="9">
         <v>15</v>
@@ -5693,27 +6025,27 @@
       </c>
       <c r="B17">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="C17">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D17">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E17">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="F17">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="G17" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>34 33 49 13 45</v>
+        <v>13 40 9 47 16</v>
       </c>
       <c r="H17" s="9">
         <v>16</v>
@@ -5725,27 +6057,27 @@
       </c>
       <c r="B18">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
+        <v>32</v>
+      </c>
+      <c r="D18">
+        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
+        <v>38</v>
+      </c>
+      <c r="E18">
+        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
         <v>36</v>
       </c>
-      <c r="C18">
-        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>10</v>
-      </c>
-      <c r="D18">
-        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>41</v>
-      </c>
-      <c r="E18">
-        <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>19</v>
-      </c>
       <c r="F18">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G18" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>25 42 43 5 11</v>
+        <v>21 36 32 26 6</v>
       </c>
       <c r="H18" s="9">
         <v>17</v>
@@ -5757,27 +6089,27 @@
       </c>
       <c r="B19">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="C19">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="D19">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="E19">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="F19">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="G19" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>29 9 5 28 38</v>
+        <v>41 31 45 7 39</v>
       </c>
       <c r="H19" s="9">
         <v>18</v>
@@ -5789,27 +6121,27 @@
       </c>
       <c r="B20">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>65</v>
+        <v>11</v>
       </c>
       <c r="C20">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="D20">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="E20">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="F20">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G20" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>29 11 41 38 29</v>
+        <v>3 5 24 12 24</v>
       </c>
       <c r="H20" s="9">
         <v>19</v>
@@ -5821,27 +6153,27 @@
       </c>
       <c r="B21">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>18</v>
+        <v>90</v>
       </c>
       <c r="C21">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D21">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="E21">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="F21">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="G21" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>13 51 10 41 8</v>
+        <v>3 31 51 21 40</v>
       </c>
       <c r="H21" s="9">
         <v>20</v>
@@ -5853,27 +6185,27 @@
       </c>
       <c r="B22">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C22">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="D22">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="E22">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F22">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="G22" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>46 17 23 50 28</v>
+        <v>43 21 23 4 21</v>
       </c>
       <c r="H22" s="9">
         <v>21</v>
@@ -5885,27 +6217,27 @@
       </c>
       <c r="B23">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C23">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D23">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="E23">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="F23">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="G23" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>32 32 4 8 7</v>
+        <v>34 46 30 18 52</v>
       </c>
       <c r="H23" s="9">
         <v>22</v>
@@ -5917,11 +6249,11 @@
       </c>
       <c r="B24">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>25</v>
+        <v>106</v>
       </c>
       <c r="G24" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>26 18 7 32 35</v>
+        <v>38 18 12 46 43</v>
       </c>
       <c r="H24" s="9">
         <v>23</v>
@@ -5933,11 +6265,11 @@
       </c>
       <c r="B25">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>101</v>
+        <v>47</v>
       </c>
       <c r="G25" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>26 22 32 27 12</v>
+        <v>11 9 12 12 48</v>
       </c>
       <c r="H25" s="9">
         <v>24</v>
@@ -5949,11 +6281,11 @@
       </c>
       <c r="B26">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="G26" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>27 12 34 25 17</v>
+        <v>7 15 47 9 18</v>
       </c>
       <c r="H26" s="9">
         <v>25</v>
@@ -5965,11 +6297,11 @@
       </c>
       <c r="B27">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="G27" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>33 28 33 38 40</v>
+        <v>12 24 34 22 36</v>
       </c>
       <c r="H27" s="9">
         <v>26</v>
@@ -5981,11 +6313,11 @@
       </c>
       <c r="B28">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="G28" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>31 41 50 24 21</v>
+        <v>26 34 31 28 31</v>
       </c>
       <c r="H28" s="9">
         <v>27</v>
@@ -5997,11 +6329,11 @@
       </c>
       <c r="B29">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="G29" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>36 44 26 12 47</v>
+        <v>31 8 47 38 10</v>
       </c>
       <c r="H29" s="9">
         <v>28</v>
@@ -6013,11 +6345,11 @@
       </c>
       <c r="B30">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>96</v>
+        <v>43</v>
       </c>
       <c r="G30" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>13 9 37 4 27</v>
+        <v>45 5 18 9 5</v>
       </c>
       <c r="H30" s="9">
         <v>29</v>
@@ -6029,11 +6361,11 @@
       </c>
       <c r="B31">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>110</v>
+        <v>28</v>
       </c>
       <c r="G31" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>46 38 17 39 41</v>
+        <v>8 12 11 39 43</v>
       </c>
       <c r="H31" s="9">
         <v>30</v>
@@ -6045,11 +6377,11 @@
       </c>
       <c r="B32">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="G32" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>13 25 30 16 40</v>
+        <v>10 45 50 18 48</v>
       </c>
       <c r="H32" s="9">
         <v>31</v>
@@ -6061,11 +6393,11 @@
       </c>
       <c r="B33">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G33" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>12 25 37 13 34</v>
+        <v>17 13 17 13 45</v>
       </c>
       <c r="H33" s="9">
         <v>32</v>
@@ -6077,11 +6409,11 @@
       </c>
       <c r="B34">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="G34" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>51 50 21 13 28</v>
+        <v>18 30 30 5 6</v>
       </c>
       <c r="H34" s="9">
         <v>33</v>
@@ -6093,11 +6425,11 @@
       </c>
       <c r="B35">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G35" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>18 22 13 10 41</v>
+        <v>8 42 8 24 42</v>
       </c>
       <c r="H35" s="9">
         <v>34</v>
@@ -6109,11 +6441,11 @@
       </c>
       <c r="B36">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>97</v>
+        <v>3</v>
       </c>
       <c r="G36" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>7 18 48 45 16</v>
+        <v>47 39 43 46 36</v>
       </c>
       <c r="H36" s="9">
         <v>35</v>
@@ -6125,11 +6457,11 @@
       </c>
       <c r="B37">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>85</v>
+        <v>6</v>
       </c>
       <c r="G37" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>39 11 41 5 50</v>
+        <v>6 14 23 52 22</v>
       </c>
       <c r="H37" s="9">
         <v>36</v>
@@ -6141,11 +6473,11 @@
       </c>
       <c r="B38">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="G38" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>24 44 33 47 9</v>
+        <v>8 26 52 25 26</v>
       </c>
       <c r="H38" s="9">
         <v>37</v>
@@ -6157,11 +6489,11 @@
       </c>
       <c r="B39">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>7</v>
+        <v>106</v>
       </c>
       <c r="G39" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>29 46 31 47 31</v>
+        <v>7 31 45 46 26</v>
       </c>
       <c r="H39" s="9">
         <v>38</v>
@@ -6173,11 +6505,11 @@
       </c>
       <c r="B40">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G40" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>8 8 8 4 40</v>
+        <v>10 18 5 27 22</v>
       </c>
       <c r="H40" s="9">
         <v>39</v>
@@ -6189,11 +6521,11 @@
       </c>
       <c r="B41">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="G41" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>34 26 36 5 11</v>
+        <v>9 49 18 19 4</v>
       </c>
       <c r="H41" s="9">
         <v>40</v>
@@ -6205,11 +6537,11 @@
       </c>
       <c r="B42">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>105</v>
+        <v>16</v>
       </c>
       <c r="G42" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>42 7 29 50 27</v>
+        <v>20 33 19 14 10</v>
       </c>
       <c r="H42" s="9">
         <v>41</v>
@@ -6221,11 +6553,11 @@
       </c>
       <c r="B43">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>95</v>
+        <v>9</v>
       </c>
       <c r="G43" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>26 37 27 18 18</v>
+        <v>40 15 30 24 16</v>
       </c>
       <c r="H43" s="9">
         <v>42</v>
@@ -6237,11 +6569,11 @@
       </c>
       <c r="B44">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G44" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>9 9 7 44 45</v>
+        <v>33 46 46 21 26</v>
       </c>
       <c r="H44" s="9">
         <v>43</v>
@@ -6253,11 +6585,11 @@
       </c>
       <c r="B45">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>81</v>
+        <v>11</v>
       </c>
       <c r="G45" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>31 13 7 44 5</v>
+        <v>45 29 14 28 32</v>
       </c>
       <c r="H45" s="9">
         <v>44</v>
@@ -6269,11 +6601,11 @@
       </c>
       <c r="B46">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="G46" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>22 12 18 48 12</v>
+        <v>49 27 39 34 17</v>
       </c>
       <c r="H46" s="9">
         <v>45</v>
@@ -6285,11 +6617,11 @@
       </c>
       <c r="B47">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="G47" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>12 24 45 46 8</v>
+        <v>40 7 30 35 39</v>
       </c>
       <c r="H47" s="9">
         <v>46</v>
@@ -6301,11 +6633,11 @@
       </c>
       <c r="B48">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="G48" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>10 11 13 7 41</v>
+        <v>45 42 6 50 3</v>
       </c>
       <c r="H48" s="9">
         <v>47</v>
@@ -6317,11 +6649,11 @@
       </c>
       <c r="B49">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="G49" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>14 49 32 20 39</v>
+        <v>23 6 13 48 7</v>
       </c>
       <c r="H49" s="9">
         <v>48</v>
@@ -6333,11 +6665,11 @@
       </c>
       <c r="B50">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="G50" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>49 10 37 42 20</v>
+        <v>39 51 26 28 42</v>
       </c>
       <c r="H50" s="9">
         <v>49</v>
@@ -6349,11 +6681,11 @@
       </c>
       <c r="B51">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G51" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>7 22 9 51 24</v>
+        <v>51 29 17 39 46</v>
       </c>
       <c r="H51" s="9">
         <v>50</v>
@@ -6365,11 +6697,11 @@
       </c>
       <c r="B52">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="G52" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>3 45 32 41 26</v>
+        <v>18 50 44 10 32</v>
       </c>
       <c r="H52" s="9">
         <v>51</v>
@@ -6381,11 +6713,11 @@
       </c>
       <c r="B53">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G53" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>42 19 31 43 18</v>
+        <v>11 37 50 17 47</v>
       </c>
       <c r="H53" s="9">
         <v>52</v>
@@ -6397,11 +6729,11 @@
       </c>
       <c r="B54">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="G54" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>43 28 13 40 5</v>
+        <v>16 29 38 48 12</v>
       </c>
       <c r="H54" s="9">
         <v>53</v>
@@ -6413,11 +6745,11 @@
       </c>
       <c r="B55">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>89</v>
+        <v>41</v>
       </c>
       <c r="G55" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>11 8 31 6 23</v>
+        <v>47 3 48 23 33</v>
       </c>
       <c r="H55" s="9">
         <v>54</v>
@@ -6429,11 +6761,11 @@
       </c>
       <c r="B56">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="G56" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>30 22 39 21 26</v>
+        <v>52 20 6 42 23</v>
       </c>
       <c r="H56" s="9">
         <v>55</v>
@@ -6445,11 +6777,11 @@
       </c>
       <c r="B57">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="G57" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>21 45 31 44 42</v>
+        <v>49 39 3 24 33</v>
       </c>
       <c r="H57" s="9">
         <v>56</v>
@@ -6461,11 +6793,11 @@
       </c>
       <c r="B58">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="G58" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>22 43 47 14 44</v>
+        <v>27 20 39 11 4</v>
       </c>
       <c r="H58" s="9">
         <v>57</v>
@@ -6477,7 +6809,7 @@
       </c>
       <c r="B59">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="H59" s="9">
         <v>58</v>
@@ -6489,7 +6821,7 @@
       </c>
       <c r="B60">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="H60" s="9">
         <v>59</v>
@@ -6501,7 +6833,7 @@
       </c>
       <c r="B61">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>110</v>
+        <v>23</v>
       </c>
       <c r="H61" s="9">
         <v>60</v>
@@ -6513,7 +6845,7 @@
       </c>
       <c r="B62">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="H62" s="9">
         <v>61</v>
@@ -6525,7 +6857,7 @@
       </c>
       <c r="B63">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="H63" s="9">
         <v>62</v>
@@ -6537,7 +6869,7 @@
       </c>
       <c r="B64">
         <f ca="1">RANDBETWEEN(MIN(School!$D:$D),MAX(School!$D:$D))</f>
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="H64" s="9">
         <v>63</v>
@@ -6848,7 +7180,7 @@
       </c>
       <c r="E2" s="6" t="str">
         <f ca="1">RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))</f>
-        <v>51 14 2</v>
+        <v>24 50 36</v>
       </c>
       <c r="F2" s="4">
         <f ca="1">RANDBETWEEN(MIN(CompetitionHost!$F:$F),MAX(CompetitionHost!$F:$F))</f>
@@ -6856,7 +7188,7 @@
       </c>
       <c r="G2" s="4" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>23 5 34 45 35 32 22 9 49 19 9 43 3</v>
+        <v>24 9 36 17 33 15 37 10 8 25 22 12 6</v>
       </c>
       <c r="H2" s="11">
         <v>1</v>
@@ -6874,7 +7206,7 @@
       </c>
       <c r="E3" s="6" t="str">
         <f ca="1">RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))</f>
-        <v>56 39 30</v>
+        <v>30 1 52</v>
       </c>
       <c r="F3" s="4">
         <f ca="1">RANDBETWEEN(MIN(CompetitionHost!$F:$F),MAX(CompetitionHost!$F:$F))</f>
@@ -6882,7 +7214,7 @@
       </c>
       <c r="G3" s="4" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>41 40 23 35 18 33 41 21 36 22 23 37 10 32 31 44 52</v>
+        <v>27 37 7 28 35 29 16 8 4 6 17 15 44 49 34 35 40</v>
       </c>
       <c r="H3" s="11">
         <v>2</v>
@@ -6960,11 +7292,11 @@
       </c>
       <c r="C2" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>40 7 19 7 12</v>
+        <v>47 21 36 3 38</v>
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))</f>
-        <v>27 13 1</v>
+        <v>54 17 30</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>343</v>
@@ -6979,11 +7311,11 @@
       </c>
       <c r="C3" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>8 38 23 30 47</v>
+        <v>46 6 20 46 6</v>
       </c>
       <c r="D3" s="6" t="str">
         <f ca="1">RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))</f>
-        <v>54 43 26</v>
+        <v>28 13 61</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>346</v>
@@ -6998,11 +7330,11 @@
       </c>
       <c r="C4" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>43 11 28 3 30</v>
+        <v>8 4 21 35 49</v>
       </c>
       <c r="D4" s="6" t="str">
         <f ca="1">RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))</f>
-        <v>25 57 18</v>
+        <v>58 28 55</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>344</v>
@@ -7017,11 +7349,11 @@
       </c>
       <c r="C5" t="str">
         <f ca="1">RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Member!$H:$H),MAX(Member!$H:$H))</f>
-        <v>52 37 48 8 25</v>
+        <v>4 48 11 31 42</v>
       </c>
       <c r="D5" s="6" t="str">
         <f ca="1">RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))&amp;" "&amp;RANDBETWEEN(MIN(Club!$H:$H),MAX(Club!$H:$H))</f>
-        <v>18 35 7</v>
+        <v>38 28 5</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>345</v>

</xml_diff>